<commit_message>
sample of new databooks for testing uploaded
</commit_message>
<xml_diff>
--- a/inputs/fr/Optima_template.xlsx
+++ b/inputs/fr/Optima_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Covid-India-UP\Nutrition\inputs\fr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{161BA057-898A-42B1-A5C6-78BFBFFDE8CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{66B084B8-C1E4-40C1-8A0D-5FC331467B07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36" yWindow="24" windowWidth="23004" windowHeight="12336" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2692,7 +2692,7 @@
       <c r="A63" s="57"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="kNkcaAGZOYzTwSI0v5X4ZkqQBGBmhxxGwUbkb+E6oAd4whRE8dbJwaxxtuceT6zaqBDFxafv3YFbbGamopreAQ==" saltValue="YJMrzFaBVMMkCdh3EsYfHQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="QJTi4/5QI+NK8kyPsACSFSrUiD/uloMWJe5VF+xH1grxIKVQpbRGlHww+4KyJctnhqj2ST/jZ5fln+2UfjQzNg==" saltValue="SEX/+lxJJaBTnduR5EwWiQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -3470,7 +3470,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="xBOfVpRpDTtlErBQCfADVaVuP1AJtJMv2wMqf3MbQPz0D9TXaaftEkTOUI0OCgp1wRuUXYkq2c2wgzINGW/5Kw==" saltValue="d7S31tRDYYxOw5Qx8Wg6dw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2Cel0n6I8tK1o6rWuJwGKl27Mazl+wlZFE4qzq2Fl4xIDplUeZeJPuicX1MzN8nE1CFH5g7doS8QTtBWswRyHQ==" saltValue="SmO8595GOnZehC0vXQKRQA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -3620,7 +3620,7 @@
       <c r="C20" s="50"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="egdQZyrZEd8QMJue4uy3M/T5rebusisUCFpXgW96rRt5XkST4G/tinZAw6SuMj8tyDKZWGtuFG5n9ZsXS9rAIg==" saltValue="lqVO4QIUd8Zrsae5d9pxJw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="3mbZOnw/f59Vq/WkcN7KpzpdLSaDMVcQUVZHLvVbPiGGxlEpHEJPqQOh18tbp6VFceHDmrSmKSgtQdcCtibPeg==" saltValue="MAxuDC6jPB9IPQR8r7FuDA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
@@ -3721,7 +3721,7 @@
       <c r="A19" s="25"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wXGkM20Pfyt4vtXWwGJKFRa0mAn3lNbaVd/9wUy7pW9bpGjiwujnaQo1GBvQRM17vfpacETmD11KcnnmEaHmww==" saltValue="FHlUjEVa7kjbt7gBI+DjEA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="eV8+Vif18beOgXXnwVyVJrY3jpgL5f7hhfT2iJi6IQVwa8ZU4qymxmER0URJUuRrpTVWJU3TjumUw4O6ERqnZg==" saltValue="ZBiox1sCmDvNAGmtbl9+cw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -3836,7 +3836,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="XLToagOKKNruY10i9bTg8jRaehOFDXeX/hPRPcF1MDiulVy3o3ZeBzWLLbbF8tiu0fanDl7n0DeNZQZoFtKs3g==" saltValue="IKjtsQWNL+AbPm48EZFz8g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Mm1xqcHLMPfGiZeX9GtxgCMatdceWr31wRSbTHS9hUda1KT6jA7fzOhFg+rkXvdHxv7uowkvrv+wfr6LL/05Mw==" saltValue="IUUk8Uz4BnPsfR+Jc1zJCw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -5597,7 +5597,7 @@
       <c r="B40" s="19"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="LO1ZYf9ctlt9jZmzChGGatp1TU0pLO7e3hbU20IsY5y5WfqwfuITJiffL1Ha9VrzQMcRsCAPvgvA7o6SkvI5OA==" saltValue="BSvG8YaDLASTSUq/tIozew==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="TqYmLdIibGUZaW4+SE0mnyDJI6BwWh8BT39Puw9s56ESdWnXngRbTDGSDNxqneQe15Zcx92O2Yiq0AixSpvNbw==" saltValue="Mytt0bEd788AVugo+wiAcQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -5632,7 +5632,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="kpBwaYNajt5wRRVxe6mUpcJwD/b1JY75nxOe6F/e4Bgel4Exp/1nqJB4F3BUqykekNwypynONCsJe8dds7dwxQ==" saltValue="FVrrrk2jicsInLPPQkx4Hg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="a/iZc2UAO69e8CV6pR7LNuwbvCJ/8jFBB7SnGhQSzQz/IhGxK8aB0K6H6+Pk0PDpswSgwubzBjAmANGr3rflTA==" saltValue="hmK2B16m/8lnHsFURcUx/g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5838,7 +5838,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="PlCNJ5v4BxeL4bzcnex6bsah53xGI/dP5OCg8newQV4KVJerpnCI2j/v5mcJm9D9Ye2GPpKKWT9bLkujl/nbEg==" saltValue="2wc3V0BF2KdCtR0zuAjJ4Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="dGKgwC/8+KBYoXScUuoTUXWu/1ac2tkANIY5iWiklVWAi8nh2AtdcnPfjyL2ERF+3zA3DMtXFnbwJuxy2erMBA==" saltValue="pU54W9wmfjwkRiUrRs4gXg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -7653,7 +7653,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/gBxK3cLhqDW1xm+/bJQJFDzBu+EInzLUxUTY3r5SDT9kBIbEiyXGG7bPgh/OUUCGZcLeM6lcB73I9gCqJVRdg==" saltValue="SmHGeaOT6eGewqifEZw1cQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="vKUS7Xj7v1txM0GfXaJIJkcdHVtRKmNPHWISGXgk7VFAkfpp4zIX5NLYF1pfMYgWNbkMF6bfEWfrwAT/j8eRjA==" saltValue="ws7rCf2nrMmRczFz+GLsbw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8421,7 +8421,7 @@
       <c r="K39" s="87"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Bhu4Qha01LaVjqfLkwGihC6x5VCPiGQhRT9dzURanwV1Zzs8LLukvJqyhbaa+XBJQBPomsHNm0PQMsDkkYPAJw==" saltValue="QG8PwPtD5uH6qIQ3L+NCyQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="G050OKa4DTF5bOWRGOHG0DnHFCgwlaW4uswzgnLS/s88w6zoTXXlVCeLQI3BSxQnilCeoYv0g3+xk7myaatEhw==" saltValue="aH8rxgZLDvxnnwNQph2icQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8796,7 +8796,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="RA4WnxtojASXrgJwVrE9SBjSd0AkEuwRApMBE6cCtTpOH+GLGIxVU6q8qpyhMM115TUBJNnrOAEmsgOalGio2w==" saltValue="Yl3A0asMijVxPM5LTR7K7Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="srxKj5v/cPLWdnGpNNB+Fk92J4GrW/jkxrTCkiBxwLx5ln8a4DJ7QgqR6ilWcsDezJDCIWfv2PmsJWQ0G6+PGw==" saltValue="Ce9lYrbLeEAnhrTdGCZ7kg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9786,7 +9786,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="yuxuDecZlulkl5EtmP/9FqdoEZEJxKmljoy2aKOJdi+OcX+pirSLYz3hN4iyYkefUdSdmvwMw5XlJX/ha9kkDw==" saltValue="zrtoafL/i9E7K/bkJd6HVQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="IX/B6VHIii+5GSR39NXNgcOIgMVCRlTtw+bgA75Xfml0xG5dopckd0lKx2zqGmbtJajSDG+TwDOVX3AbEz+//g==" saltValue="f8I1d1UncK3nTIlTjKx2EA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="B2:I16 B18:I40 B17:C17 E17:I17">
     <cfRule type="expression" dxfId="0" priority="9">
       <formula>$A2=""</formula>
@@ -13604,7 +13604,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="D1BNVU5c29szf5NPI03HCXfjp9t9eL5fnGYJ7qp3p6jmqP/ZItC2LLrVdJUvjYntjYOykIEhoOC5DbJ7fSstig==" saltValue="dMGFxhNtv2q8M8YYThfL+A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="0CPpy6LkQC1zeEB12pVseo/D6mg3NExp1n8XP5nv45B78VAR93bpbwvduFeZEjClg7CQrbwwIFJ+qTwnNp/QQQ==" saltValue="/PWonnJJDuy69MWZYrPDrg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="45">
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B2:B4"/>
@@ -14871,7 +14871,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="NyuS8R1pBwYzF/LxYh2f+KgdTMFRBzOB0+i1+FTF9KrEEPR7gcq3gfOhw9CowNOOOCNMjRuGGTnJ9X/KwXbUwQ==" saltValue="VEwDrqC7KQT8+1O1vXQd/g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="06m/efVQ74LwCu0KDd09ZY5g1UerE2lz9+hm66LdPV4dMNNq94SpYaMMd2bpORyZ6AS9f+5lWkbinLpezDw5Ag==" saltValue="BI9Dr48hBMivCxocGENSJA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -23010,7 +23010,7 @@
       <c r="I328" s="77"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="F7GxJ1X5z0/GuYzz6UNJWbQeo6mj7rGbD/UkhhPh7tKdXFHE9c/NqFI3OjjDd2b9uCZ1IAE5ex6Fgm0iiNeQEw==" saltValue="oRo8dNFDZXA/aHnWaF0BRg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="REAOKAx6HGfABkbs17LkjXA1bdIFYxFbJvuGqmZwGAlv+Y9B5YXJohI9p80apdMHuYM4FR3rzmXXddCP3e8TTQ==" saltValue="Q8HGALDAiIR1c1BBOn9FSw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -24100,7 +24100,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="T7WUV+pnS4bZbL5tv+jGDfmU1rlVZ1TixpV0hNyDHNVbAk2in6P2g50DL9QnFcjxSIuymZCLDBl/n4TzERA3Og==" saltValue="Ns2Y5NLD1vlgN/Y9CB+kYg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2M2+lYOaJ+mg8cjAkRDRrnlZQ9WcICQlepLUWOfF3aPQsGttDc5LBWSBPpTWppRzvzOYgbvg59OKCaaEQ8LPOQ==" saltValue="s37Uz8lgKwJPppfKgSyH7Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -24972,7 +24972,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KEIkea3mDFPRuCthRw7aeue0+7IqsAfMAD53D1hzmsmqt1DY1VOhAoS29Xkew3CsDE53th2bAFBpg50uZp9GXg==" saltValue="1He5CIW355LfBvN2VLKgMg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="25UISFydgwbjb4q4le29ejJH5OjG66Z5/S8KuaVq9AoHmtRlyAsJZGVvLiZEz6tAia/xh3W+0gZ21VcVk5gaoQ==" saltValue="5pb5w/LYB+9ogQBDbjYV9w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -27857,7 +27857,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DfXHOZsN/KqoVMKhgVUK+vQfXiTa4rgDenMOe4VUoxkgq9JhYiCebNNrXui/OpknKU6YoAArMegXLvgAyA03Fg==" saltValue="JgEtyYSNZZiVUwn6nYrscg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Mr+5mXUObzeL0crKfR0QG+H32m11xxq0uChJqTqMQ8jxAbgWhL8j1jRmEgCcK2ct8Um888AQP20OOQZ5vWhIrA==" saltValue="b9V646B55dK7ikwjZfJEUg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -28139,7 +28139,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="pancduqDo4CVgGsALkA984WhfWdgAwBXJSuQkCoQx3SgEeeI96kheooKE2pbWbn7IZM95oa5rGcrCCWOJHD6dg==" saltValue="Cq0dgUNWGEdLOOCCtHp1iQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Qbi0E7dL0s3yJFRHXhQusvJlb/Y2fmLCeQpheqcrgp2rE9bg80AfJOWlFhnhen/cIqRzO15WzweGN6PYbZdOIw==" saltValue="JZvH8sxq7hzJl6HfbRmLJQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -32254,7 +32254,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9HWPkCyfJ+U0EzbRXSr9Nwx/xpPFtNyddaph5k86xj2DYG5KF69NEkxr6zt6KxYRuZKgtR0/406G4ILw+BIEZw==" saltValue="eEZwr3/7XHutXMu3T6tSyQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="q/luzU6ArjrzPGS8B5BzFLUQRTMI5MD9c8PG3GTE/iovCQFW1IBgid9h2Ln2zWdhVdgG/tA0plBVxiOfU4IaRw==" saltValue="oNwWtYXK4zfXpY8U/0YmLw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -32770,7 +32770,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="3AAokZM4jJUtpj8fVmQpoKtplnMEawv/PjGyD+W2y+h7BnrS2JFAQbOg45p+nMMoPXd4rUdOzGrGgi146+jPrg==" saltValue="ptZRnOhku+iCPzX25ag5cA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="HpnhKU+Sg7mMchUGiE8eiEZzW/lkl6OQR5GrP7lkHtT60x88XFSfRD/u6fvHgZAZFENXZQkytj8SngWuyeXutg==" saltValue="rN6eGAsXuTbtz6cup+3Q4A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -33101,7 +33101,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="N/6TFaCoEC+K+bnMWRnkqsKJ2juUgIIbJJiybLBca4XHyoaTMSjYgPryO3JI0PU8XwYg8jM85hX0reoT4WH/Ug==" saltValue="8eDVTq2BSc60hc4Cmzdl0A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="FEvp3E1K/UjOdCn0t61+Gdp24s/bNilL9ExXNvo0LgsiXOzFuUROd/uOoi6QwkA5cJMLYgPuKGR1DjzJl519tA==" saltValue="LJGrAVa42iH3Jn27dC+ALg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -33359,7 +33359,7 @@
       <c r="G17" s="3"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="dMvju11IS2hBfn0j8nVKzFFLpCMkD6sqkDVjJyy2DCN88pvdeQmktK8AoN8UtkbQMqK9plK/C14geogH3cld8Q==" saltValue="mZt3wsvHicId3FlrOnBZBw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="hr85/gpEzQpOJMonXZjmd1zkhy/FoIGNjrEJV8GUYGTOsr5BBBSKa4rmJmtthRsrY+xFqdrK+9vLLaRZ2APt1A==" saltValue="hpeKUqIjJ/0VZiNP1p3olA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -33450,7 +33450,7 @@
       <c r="G5" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="l5HsOcAmpQzmo2l1Cqu4hp+SiSkeTshDoX3jOLjmHWkkuzY1pYC4w48qLPKfH14Wz+IvTRTTfFJmW/xMNodNhA==" saltValue="beNraHIcVfkUhMuK8iH8xQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ScW+dH3YWedluddHWszqxi3wsWmLThWuB6YFXupjP9LQmIiFHFf1GzO2t2dclArTMKVpg1gZgZetMFMZOZO6OA==" saltValue="Ou/AWTkyRazGJMd70KdyMQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -33678,7 +33678,7 @@
       <c r="L14" s="103"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="GkPw3CuECrZ83SMB2+U3z+0wNh8xAaidu3wHD2W+3BGgN04Q4jip8KTv0hYAg8Phf3dXHgFBU0HmQvw6lLkpBQ==" saltValue="E8m8rjgq9y8zEchAbG6zOA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="bRlU+5L5pcKaa4QwjlO0TUBzmGr6jT/uRgKhYs3w7woIno8Fxq6nnVpXX6uwDvFMCXFARQREq/KM1wiOkcth4Q==" saltValue="dHvU1rMKAA+iwuLoxffoOg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="193" orientation="portrait"/>
 </worksheet>
@@ -33756,7 +33756,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="tXsxZPoujV7tmajan0gTSJ/AQv4A1px2RPTxdDazhfGq2HTplu0DVnfe96OvlGtuQjoPBOHq1JzAhGmcSjfpIQ==" saltValue="PnxFa5FprLHjFbI8Nhk+EQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Chl7ZeHsHL1683Rlsjq6QJNHHLorT3qKd03CD/vk+vqKBmdnwK+HEM7yDkqyVRKnDuMmEqZpWlF9PhJ1LynQwg==" saltValue="RYWwx0EjWdZPYyTnfPx3LQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -34019,7 +34019,7 @@
       <c r="E21" s="47"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+T5Agrk8H0rFhOWENWPYS6hmtoanELw0qSANblezucmWGa6WILv+qIgrsry1v9kzNX3KSKKp1Yh0WKe0bBkTqg==" saltValue="gIWd0NvJ4bLDNd2gTgOLaQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="iTJ5HoqC49WyEaKKiKnQQF0GbtmllLpkyNGJAq/fjddw4o9t/B1VtE8on7afKd5IsasXrNQonOQf6r7jTBoDfg==" saltValue="mm/jxzg1tCUWJ/hDGpAyTw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -34083,7 +34083,7 @@
       <c r="D3" s="47"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9DEnaO33j/f7rxANX9s1wQ23NP/vfwQfPs+FNlV0qieGakHqWLUpuHWZvKPRfptERGXrDvl1KfXK90TnkuwqlQ==" saltValue="HTxcKpfXP+eA3fZB9P2KfA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="mufbpzKK2aKFj09cgeSzW+TCevWodNjkOqG1eUMxYBG7nMcQPJJ8ZTwGzLXFyIPpxn0Qu9fuc11cXx6KI9LvBA==" saltValue="tLqqpsZSHy3S4vjaQ8PpQg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Decrease font size on cause of death sheet
</commit_message>
<xml_diff>
--- a/inputs/fr/Optima_template.xlsx
+++ b/inputs/fr/Optima_template.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aimee.altermatt\Documents\GitHub\Nutrition\inputs\fr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B4A98D4-5153-4C8A-BFF7-7B7296AFDD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7556B9F9-4A02-4EA5-A1A5-1B8B2589AAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="50" yWindow="740" windowWidth="19150" windowHeight="10060" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15795" yWindow="-15840" windowWidth="21600" windowHeight="12525" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Donnees pop de l'annee de ref" sheetId="1" r:id="rId1"/>
+    <sheet name="Données pop de l'année de ref" sheetId="1" r:id="rId1"/>
     <sheet name="Projections démographiques" sheetId="2" r:id="rId2"/>
     <sheet name="Causes du décès" sheetId="3" r:id="rId3"/>
     <sheet name="Dist. de l'état nutritionnel" sheetId="4" r:id="rId4"/>
@@ -43,53 +43,53 @@
     <sheet name="Programmes pour les FE" sheetId="28" state="hidden" r:id="rId28"/>
   </sheets>
   <definedNames>
-    <definedName name="abortion" localSheetId="7">'Donnees pop de l''annee de ref'!$C$38</definedName>
-    <definedName name="abortion">'Donnees pop de l''annee de ref'!$C$41</definedName>
+    <definedName name="abortion" localSheetId="7">'Données pop de l''année de ref'!$C$38</definedName>
+    <definedName name="abortion">'Données pop de l''année de ref'!$C$41</definedName>
     <definedName name="comm_deliv">'Traitement de la MAS'!$D$3</definedName>
-    <definedName name="diarrhoea_1_5mo">'Donnees pop de l''annee de ref'!$C$52</definedName>
-    <definedName name="diarrhoea_12_23mo">'Donnees pop de l''annee de ref'!$C$54</definedName>
-    <definedName name="diarrhoea_1mo">'Donnees pop de l''annee de ref'!$C$51</definedName>
-    <definedName name="diarrhoea_24_59mo">'Donnees pop de l''annee de ref'!$C$55</definedName>
-    <definedName name="diarrhoea_6_11mo">'Donnees pop de l''annee de ref'!$C$53</definedName>
-    <definedName name="end_year">'Donnees pop de l''annee de ref'!$C$4</definedName>
-    <definedName name="famplan_unmet_need">'Donnees pop de l''annee de ref'!$C$13</definedName>
-    <definedName name="food_insecure">'Donnees pop de l''annee de ref'!$C$8</definedName>
-    <definedName name="frac_children_health_facility">'Donnees pop de l''annee de ref'!$C$12</definedName>
-    <definedName name="frac_diarrhea_severe">'Donnees pop de l''annee de ref'!$C$58</definedName>
-    <definedName name="frac_maize">'Donnees pop de l''annee de ref'!$C$19</definedName>
-    <definedName name="frac_malaria_risk">'Donnees pop de l''annee de ref'!$C$9</definedName>
+    <definedName name="diarrhoea_1_5mo">'Données pop de l''année de ref'!$C$52</definedName>
+    <definedName name="diarrhoea_12_23mo">'Données pop de l''année de ref'!$C$54</definedName>
+    <definedName name="diarrhoea_1mo">'Données pop de l''année de ref'!$C$51</definedName>
+    <definedName name="diarrhoea_24_59mo">'Données pop de l''année de ref'!$C$55</definedName>
+    <definedName name="diarrhoea_6_11mo">'Données pop de l''année de ref'!$C$53</definedName>
+    <definedName name="end_year">'Données pop de l''année de ref'!$C$4</definedName>
+    <definedName name="famplan_unmet_need">'Données pop de l''année de ref'!$C$13</definedName>
+    <definedName name="food_insecure">'Données pop de l''année de ref'!$C$8</definedName>
+    <definedName name="frac_children_health_facility">'Données pop de l''année de ref'!$C$12</definedName>
+    <definedName name="frac_diarrhea_severe">'Données pop de l''année de ref'!$C$58</definedName>
+    <definedName name="frac_maize">'Données pop de l''année de ref'!$C$19</definedName>
+    <definedName name="frac_malaria_risk">'Données pop de l''année de ref'!$C$9</definedName>
     <definedName name="frac_mam_1_5months">'Dist. de l''état nutritionnel'!$D$10</definedName>
     <definedName name="frac_mam_12_23months">'Dist. de l''état nutritionnel'!$F$10</definedName>
     <definedName name="frac_mam_1month">'Dist. de l''état nutritionnel'!$C$10</definedName>
     <definedName name="frac_mam_24_59months">'Dist. de l''état nutritionnel'!$G$10</definedName>
     <definedName name="frac_mam_6_11months">'Dist. de l''état nutritionnel'!$E$10</definedName>
-    <definedName name="frac_MAMtoSAM">'Donnees pop de l''annee de ref'!#REF!</definedName>
-    <definedName name="frac_other_staples">'Donnees pop de l''annee de ref'!$C$20</definedName>
-    <definedName name="frac_PW_health_facility">'Donnees pop de l''annee de ref'!$C$11</definedName>
-    <definedName name="frac_rice">'Donnees pop de l''annee de ref'!$C$17</definedName>
+    <definedName name="frac_MAMtoSAM">'Données pop de l''année de ref'!#REF!</definedName>
+    <definedName name="frac_other_staples">'Données pop de l''année de ref'!$C$20</definedName>
+    <definedName name="frac_PW_health_facility">'Données pop de l''année de ref'!$C$11</definedName>
+    <definedName name="frac_rice">'Données pop de l''année de ref'!$C$17</definedName>
     <definedName name="frac_sam_1_5months">'Dist. de l''état nutritionnel'!$D$11</definedName>
     <definedName name="frac_sam_12_23months">'Dist. de l''état nutritionnel'!$F$11</definedName>
     <definedName name="frac_sam_1month">'Dist. de l''état nutritionnel'!$C$11</definedName>
     <definedName name="frac_sam_24_59months">'Dist. de l''état nutritionnel'!$G$11</definedName>
     <definedName name="frac_sam_6_11months">'Dist. de l''état nutritionnel'!$E$11</definedName>
-    <definedName name="frac_SAMtoMAM">'Donnees pop de l''annee de ref'!#REF!</definedName>
-    <definedName name="frac_subsistence_farming">'Donnees pop de l''annee de ref'!$C$16</definedName>
-    <definedName name="frac_wheat">'Donnees pop de l''annee de ref'!$C$18</definedName>
-    <definedName name="infant_mortality">'Donnees pop de l''annee de ref'!$C$38</definedName>
-    <definedName name="iron_deficiency_anaemia">'Donnees pop de l''annee de ref'!$C$59</definedName>
+    <definedName name="frac_SAMtoMAM">'Données pop de l''année de ref'!#REF!</definedName>
+    <definedName name="frac_subsistence_farming">'Données pop de l''année de ref'!$C$16</definedName>
+    <definedName name="frac_wheat">'Données pop de l''année de ref'!$C$18</definedName>
+    <definedName name="infant_mortality">'Données pop de l''année de ref'!$C$38</definedName>
+    <definedName name="iron_deficiency_anaemia">'Données pop de l''année de ref'!$C$59</definedName>
     <definedName name="manage_mam">'Traitement de la MAS'!$D$2</definedName>
-    <definedName name="maternal_mortality">'Donnees pop de l''annee de ref'!$C$40</definedName>
-    <definedName name="neonatal_mortality">'Donnees pop de l''annee de ref'!$C$37</definedName>
-    <definedName name="Percentage_of_pregnant_women_attending_health_facility">'Donnees pop de l''annee de ref'!$C$11</definedName>
-    <definedName name="preterm_AGA">'Donnees pop de l''annee de ref'!$C$46</definedName>
-    <definedName name="preterm_SGA">'Donnees pop de l''annee de ref'!$C$45</definedName>
-    <definedName name="school_attendance">'Donnees pop de l''annee de ref'!$C$10</definedName>
-    <definedName name="start_year">'Donnees pop de l''annee de ref'!$C$3</definedName>
-    <definedName name="stillbirth" localSheetId="7">'Donnees pop de l''annee de ref'!$C$39</definedName>
-    <definedName name="stillbirth">'Donnees pop de l''annee de ref'!$C$42</definedName>
-    <definedName name="term_AGA">'Donnees pop de l''annee de ref'!$C$48</definedName>
-    <definedName name="term_SGA">'Donnees pop de l''annee de ref'!$C$47</definedName>
-    <definedName name="U5_mortality">'Donnees pop de l''annee de ref'!$C$39</definedName>
+    <definedName name="maternal_mortality">'Données pop de l''année de ref'!$C$40</definedName>
+    <definedName name="neonatal_mortality">'Données pop de l''année de ref'!$C$37</definedName>
+    <definedName name="Percentage_of_pregnant_women_attending_health_facility">'Données pop de l''année de ref'!$C$11</definedName>
+    <definedName name="preterm_AGA">'Données pop de l''année de ref'!$C$46</definedName>
+    <definedName name="preterm_SGA">'Données pop de l''année de ref'!$C$45</definedName>
+    <definedName name="school_attendance">'Données pop de l''année de ref'!$C$10</definedName>
+    <definedName name="start_year">'Données pop de l''année de ref'!$C$3</definedName>
+    <definedName name="stillbirth" localSheetId="7">'Données pop de l''année de ref'!$C$39</definedName>
+    <definedName name="stillbirth">'Données pop de l''année de ref'!$C$42</definedName>
+    <definedName name="term_AGA">'Données pop de l''année de ref'!$C$48</definedName>
+    <definedName name="term_SGA">'Données pop de l''année de ref'!$C$47</definedName>
+    <definedName name="U5_mortality">'Données pop de l''année de ref'!$C$39</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1428,7 +1428,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1544,6 +1544,12 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1689,7 +1695,7 @@
     <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1935,6 +1941,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2701,7 +2710,7 @@
       <c r="A63" s="52"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="gelkmODFofzP1pcdo6UFGS4NM22fBUJcos0OtoQAEJTuicABZhMn0ZKFDuKQY3s+khbLDOh9wWbjiol8WMKknw==" saltValue="0ur8T6Mz0uTmLuIQ0SppmA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="eQwhegixl60HMlJR8z6uoOe5Yle0I7tFCYzTTXTXuoTGXFwqFGVj7pB7MJpelYSpPLe0niBjlUwsiWzuRkvGKg==" saltValue="j0ihlDInsunWUibZhP+YJg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -3479,7 +3488,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="pmHVsvuYIrpeclAoT4Ov2u0d7Z+AEfg2Sw19nfU7U7gsGYzsJ52+SkO8ijUbaG4Mr1M+fR3QyVbUYU3HrXHDZQ==" saltValue="hk9KBongsDQdxIXCzTAqKw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="nMZB9ovAFO8B6IQhBGOAqg00zzy15zLrtl3PBbou6tAufSumMP0ikp4zdFCq9uqRdk6zzbDk0lPImj8QHfizfA==" saltValue="77WUXacvqusnBje/6AdDYw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -3517,7 +3526,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="44" t="s">
         <v>180</v>
       </c>
@@ -3526,7 +3535,7 @@
       </c>
       <c r="C2" s="42"/>
     </row>
-    <row r="3" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="44" t="s">
         <v>181</v>
       </c>
@@ -3535,7 +3544,7 @@
       </c>
       <c r="C3" s="42"/>
     </row>
-    <row r="4" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="44" t="s">
         <v>192</v>
       </c>
@@ -3544,7 +3553,7 @@
       </c>
       <c r="C4" s="42"/>
     </row>
-    <row r="5" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="44" t="s">
         <v>189</v>
       </c>
@@ -3553,83 +3562,83 @@
       </c>
       <c r="C5" s="42"/>
     </row>
-    <row r="6" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="44"/>
       <c r="B6" s="45"/>
       <c r="C6" s="45"/>
     </row>
-    <row r="7" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="44"/>
       <c r="B7" s="45"/>
       <c r="C7" s="45"/>
     </row>
-    <row r="8" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="44"/>
       <c r="B8" s="45"/>
       <c r="C8" s="45"/>
     </row>
-    <row r="9" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="44"/>
       <c r="B9" s="45"/>
       <c r="C9" s="45"/>
     </row>
-    <row r="10" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="44"/>
       <c r="B10" s="45"/>
       <c r="C10" s="45"/>
     </row>
-    <row r="11" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="46"/>
       <c r="B11" s="45"/>
       <c r="C11" s="45"/>
     </row>
-    <row r="12" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="46"/>
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
     </row>
-    <row r="13" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="46"/>
       <c r="B13" s="45"/>
       <c r="C13" s="45"/>
     </row>
-    <row r="14" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="46"/>
       <c r="B14" s="45"/>
       <c r="C14" s="45"/>
     </row>
-    <row r="15" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="46"/>
       <c r="B15" s="45"/>
       <c r="C15" s="45"/>
     </row>
-    <row r="16" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="46"/>
       <c r="B16" s="45"/>
       <c r="C16" s="45"/>
     </row>
-    <row r="17" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="46"/>
       <c r="B17" s="45"/>
       <c r="C17" s="45"/>
     </row>
-    <row r="18" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="46"/>
       <c r="B18" s="45"/>
       <c r="C18" s="45"/>
     </row>
-    <row r="19" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="44"/>
       <c r="B19" s="45"/>
       <c r="C19" s="45"/>
     </row>
-    <row r="20" spans="1:3" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="44"/>
       <c r="B20" s="45"/>
       <c r="C20" s="45"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="6v3M4x32+Ts5LOmvtlTnH/XauReUkuYrPJlcGk0UEmmdYkFpHNT/KBerk6d8PorsApP9n14liqMtUFxgWRTzVw==" saltValue="qtqzwj60gZwHOz50cnvbLw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Qyb5nuWFJHgXcyxWXRKwdgsoxA8ylaiP/78nsQ2BisB6jAeGqVR24k4nS5zAxp9cLx+fcxwhJYFQTPYl17BjXw==" saltValue="YaiEOdA/S7OEIsnB9aqBlw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
@@ -3659,78 +3668,78 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="23"/>
     </row>
-    <row r="11" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="23"/>
     </row>
-    <row r="12" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="23"/>
     </row>
-    <row r="13" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="23"/>
     </row>
-    <row r="14" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="23"/>
     </row>
-    <row r="15" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="23"/>
     </row>
-    <row r="16" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="23"/>
     </row>
-    <row r="17" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="23"/>
     </row>
-    <row r="18" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="23"/>
     </row>
-    <row r="19" spans="1:1" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="23"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="mDEA3YcUSvodKqBvPqfl+9xHbFyAvJhQZ41aDPUackYK2035fWfQVn66+PDndy7oN6sgPkyBKqABFYcL/zG0LQ==" saltValue="04pPSBPSGzM5W8WXN5sDvw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="yz4/ms8nwmcuHGbCXOJxw6LaoKSBXDutxKNbvnn/bkfwJzp6IRsgJnUHaLDDkV6FFCAJJ1AvER51s9WHa6PSCA==" saltValue="qi9HbfEB45btUXc3D/Ae/w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -3774,23 +3783,23 @@
         <v>87</v>
       </c>
       <c r="B2" s="13">
-        <f>'Donnees pop de l''annee de ref'!C51</f>
+        <f>'Données pop de l''année de ref'!C51</f>
         <v>0</v>
       </c>
       <c r="C2" s="13">
-        <f>'Donnees pop de l''annee de ref'!C52</f>
+        <f>'Données pop de l''année de ref'!C52</f>
         <v>0</v>
       </c>
       <c r="D2" s="13">
-        <f>'Donnees pop de l''annee de ref'!C53</f>
+        <f>'Données pop de l''année de ref'!C53</f>
         <v>0</v>
       </c>
       <c r="E2" s="13">
-        <f>'Donnees pop de l''annee de ref'!C54</f>
+        <f>'Données pop de l''année de ref'!C54</f>
         <v>0</v>
       </c>
       <c r="F2" s="13">
-        <f>'Donnees pop de l''annee de ref'!C55</f>
+        <f>'Données pop de l''année de ref'!C55</f>
         <v>0</v>
       </c>
     </row>
@@ -3845,7 +3854,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="7PCNOl9iDvel58KgmZS1u60W2WuHBUIfLSEA83TOILzd2xYoSbBE6wxce/mIRiYSmuKrH1zZay96iFMxj77u6w==" saltValue="yLwFf9nA3MB6FZIqovPvpg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="0cbPhgles/35rIWmE2TMXQeZfi4gPcq1teBriYUgp9j4gdt/8+3SMAtl55q5Q9pct173YkhG+D7mZF5OsMM7Nw==" saltValue="/Lo83NDeBoTjXhBhNk4/Ig==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -5606,7 +5615,7 @@
       <c r="B40" s="17"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="j9FDwKniSpwtEYATTBWnwRMhCWkHat8q4qedlbUp+iLMwgPA0/3b3fjS2xvO9rCQRt3EP5n4aMTVjz22BBUPHA==" saltValue="jZbOLYkeI+lqqKUcSDgo2w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="LKDG1D/LvR440iDGcYsh4ZuAgJKIwzoxygG9ZFx6CkD4SUDY+r++IIuqNETmozCU7c9x0jip0x37dMO0Q/RlDw==" saltValue="H6yAZe4Zy5CCM7j+BbRdrQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -5641,7 +5650,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="cAKfLEECVNnwTMnGFiX74CiBFAeGD9xel+ydM2m3VWQDyeNyyJgBKEBNi/0ziKmbzDOgvVgCwnNgWn3efnPTXA==" saltValue="YlA5B66kDo7CAY2FAb+0Rw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2O4m0WXTD9DFJY09SNnRWEPLg4jSDsXp7FoZxv0/P3ZgGhgoj34PdxBH7j7EY9ne7ABuD1Etr8Riu2jbKz+rFw==" saltValue="R60W6Mnm0PJCZ/ugLecmnQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5847,7 +5856,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="pF5wFOwUOK9eYR/6WQHDhDr/4wCb1S/T+316ARraVbMNiK64NQG7ubt5OEno9DGFA0Jtb1UUoG/jg/YjyisGUw==" saltValue="W4n/LkH8fzxM1gGZ+4/qoA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="tc5Dc+rj4+qS9sFTcLbHTZENeLnVT2mVZ0MaD2SdguumJeNH9GV4OgWUseVEl2C0cExpjwoLkBcK+bgQft9Gig==" saltValue="2yD9n5At1XXbLIAjeU4mCg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -7662,7 +7671,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="p1x3eUVtCJDGAyJyTAq3T1NWVs2A+Mm46mSvW+MuC6KVK0gx5ikIu+6WGyDreY9yF11/HsjJRra5qcdJOfeu2A==" saltValue="kZcD4eBnf9rl4fkVg+U4EQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="5PYa2zm1r4/9GPXtrUnRbiGk9BCIdyh+2UGQCce7EftubCRYq9PG1RPIWPh8uVt4XtELWK/OcCYIiMpzyhA17A==" saltValue="9vmNRAE3QlGabf+uPWwx3w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7729,7 +7738,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
         <v>168</v>
       </c>
@@ -7746,7 +7755,7 @@
       <c r="J2" s="82"/>
       <c r="K2" s="82"/>
     </row>
-    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="69" t="s">
         <v>169</v>
       </c>
@@ -7763,7 +7772,7 @@
       <c r="J3" s="82"/>
       <c r="K3" s="82"/>
     </row>
-    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
         <v>170</v>
       </c>
@@ -7780,7 +7789,7 @@
       <c r="J4" s="82"/>
       <c r="K4" s="82"/>
     </row>
-    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
         <v>171</v>
       </c>
@@ -7797,7 +7806,7 @@
       <c r="J5" s="82"/>
       <c r="K5" s="82"/>
     </row>
-    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="69" t="s">
         <v>172</v>
       </c>
@@ -7816,7 +7825,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="69" t="s">
         <v>173</v>
       </c>
@@ -7835,7 +7844,7 @@
       <c r="J7" s="82"/>
       <c r="K7" s="82"/>
     </row>
-    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="69" t="s">
         <v>174</v>
       </c>
@@ -7854,7 +7863,7 @@
       <c r="J8" s="82"/>
       <c r="K8" s="82"/>
     </row>
-    <row r="9" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="69" t="s">
         <v>175</v>
       </c>
@@ -7873,7 +7882,7 @@
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
     </row>
-    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="65" t="s">
         <v>176</v>
       </c>
@@ -7890,7 +7899,7 @@
       <c r="J10" s="82"/>
       <c r="K10" s="82"/>
     </row>
-    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="65" t="s">
         <v>177</v>
       </c>
@@ -7907,7 +7916,7 @@
       <c r="J11" s="82"/>
       <c r="K11" s="82"/>
     </row>
-    <row r="12" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="65" t="s">
         <v>178</v>
       </c>
@@ -7924,7 +7933,7 @@
       <c r="J12" s="82"/>
       <c r="K12" s="82"/>
     </row>
-    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="65" t="s">
         <v>179</v>
       </c>
@@ -7941,7 +7950,7 @@
       <c r="J13" s="82"/>
       <c r="K13" s="82"/>
     </row>
-    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="69" t="s">
         <v>180</v>
       </c>
@@ -7960,7 +7969,7 @@
       <c r="J14" s="82"/>
       <c r="K14" s="82"/>
     </row>
-    <row r="15" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="69" t="s">
         <v>181</v>
       </c>
@@ -7979,7 +7988,7 @@
       <c r="J15" s="82"/>
       <c r="K15" s="82"/>
     </row>
-    <row r="16" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="69" t="s">
         <v>182</v>
       </c>
@@ -8000,7 +8009,7 @@
       <c r="J16" s="82"/>
       <c r="K16" s="82"/>
     </row>
-    <row r="17" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="69" t="s">
         <v>183</v>
       </c>
@@ -8017,7 +8026,7 @@
       <c r="J17" s="82"/>
       <c r="K17" s="82"/>
     </row>
-    <row r="18" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="69" t="s">
         <v>157</v>
       </c>
@@ -8036,7 +8045,7 @@
       <c r="J18" s="82"/>
       <c r="K18" s="82"/>
     </row>
-    <row r="19" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
         <v>158</v>
       </c>
@@ -8055,7 +8064,7 @@
       <c r="J19" s="82"/>
       <c r="K19" s="82"/>
     </row>
-    <row r="20" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
         <v>159</v>
       </c>
@@ -8074,7 +8083,7 @@
       <c r="J20" s="82"/>
       <c r="K20" s="82"/>
     </row>
-    <row r="21" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="69" t="s">
         <v>184</v>
       </c>
@@ -8093,7 +8102,7 @@
       <c r="J21" s="82"/>
       <c r="K21" s="82"/>
     </row>
-    <row r="22" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="69" t="s">
         <v>185</v>
       </c>
@@ -8114,7 +8123,7 @@
       <c r="J22" s="82"/>
       <c r="K22" s="82"/>
     </row>
-    <row r="23" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="69" t="s">
         <v>186</v>
       </c>
@@ -8133,7 +8142,7 @@
       <c r="J23" s="82"/>
       <c r="K23" s="82"/>
     </row>
-    <row r="24" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="69" t="s">
         <v>187</v>
       </c>
@@ -8150,7 +8159,7 @@
       <c r="J24" s="82"/>
       <c r="K24" s="82"/>
     </row>
-    <row r="25" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="69" t="s">
         <v>188</v>
       </c>
@@ -8167,7 +8176,7 @@
       <c r="J25" s="82"/>
       <c r="K25" s="82"/>
     </row>
-    <row r="26" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="69" t="s">
         <v>189</v>
       </c>
@@ -8184,7 +8193,7 @@
       <c r="J26" s="82"/>
       <c r="K26" s="82"/>
     </row>
-    <row r="27" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="69" t="s">
         <v>190</v>
       </c>
@@ -8203,7 +8212,7 @@
       <c r="J27" s="82"/>
       <c r="K27" s="82"/>
     </row>
-    <row r="28" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="69" t="s">
         <v>191</v>
       </c>
@@ -8220,7 +8229,7 @@
       <c r="J28" s="82"/>
       <c r="K28" s="82"/>
     </row>
-    <row r="29" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="69" t="s">
         <v>192</v>
       </c>
@@ -8239,7 +8248,7 @@
       <c r="J29" s="82"/>
       <c r="K29" s="82"/>
     </row>
-    <row r="30" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="69" t="s">
         <v>205</v>
       </c>
@@ -8260,7 +8269,7 @@
       <c r="J30" s="82"/>
       <c r="K30" s="82"/>
     </row>
-    <row r="31" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="69" t="s">
         <v>161</v>
       </c>
@@ -8277,7 +8286,7 @@
       <c r="J31" s="82"/>
       <c r="K31" s="82"/>
     </row>
-    <row r="32" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="69" t="s">
         <v>193</v>
       </c>
@@ -8296,7 +8305,7 @@
       <c r="J32" s="82"/>
       <c r="K32" s="82"/>
     </row>
-    <row r="33" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="69" t="s">
         <v>194</v>
       </c>
@@ -8315,7 +8324,7 @@
       <c r="J33" s="82"/>
       <c r="K33" s="82"/>
     </row>
-    <row r="34" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="69" t="s">
         <v>195</v>
       </c>
@@ -8334,7 +8343,7 @@
       <c r="J34" s="82"/>
       <c r="K34" s="82"/>
     </row>
-    <row r="35" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="69" t="s">
         <v>196</v>
       </c>
@@ -8353,7 +8362,7 @@
       <c r="J35" s="82"/>
       <c r="K35" s="82"/>
     </row>
-    <row r="36" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="69" t="s">
         <v>197</v>
       </c>
@@ -8372,7 +8381,7 @@
       <c r="J36" s="82"/>
       <c r="K36" s="82"/>
     </row>
-    <row r="37" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="69" t="s">
         <v>198</v>
       </c>
@@ -8391,7 +8400,7 @@
       <c r="J37" s="82"/>
       <c r="K37" s="82"/>
     </row>
-    <row r="38" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="69" t="s">
         <v>199</v>
       </c>
@@ -8408,7 +8417,7 @@
       <c r="J38" s="82"/>
       <c r="K38" s="82"/>
     </row>
-    <row r="39" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="69" t="s">
         <v>200</v>
       </c>
@@ -8430,7 +8439,7 @@
       <c r="K39" s="82"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="E5AJ4+ic+Mc6pOwasiPPKnpMe1PQgtH7B5q+jXNMBumiU4a3uYKBY3aj60l5KotnBafsu4aUFMdMuSHH67IqjQ==" saltValue="VeW5TSbOiCyD+cW8FgH9Lw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="aCxXe5vwZOf0qXV1QGsIcBTMw9eephIdMh0qC0mrjM/pv/5mPW7txC23aFHpj4mM7E4EI2jZXTDAGRUhNgMMGA==" saltValue="tfnGRLgUku5FK2z4m2lA6A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8497,7 +8506,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="96" t="s">
         <v>109</v>
       </c>
@@ -8526,7 +8535,7 @@
       <c r="J2" s="82"/>
       <c r="K2" s="82"/>
     </row>
-    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="96" t="s">
         <v>96</v>
       </c>
@@ -8555,7 +8564,7 @@
       <c r="J3" s="82"/>
       <c r="K3" s="82"/>
     </row>
-    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="96" t="s">
         <v>97</v>
       </c>
@@ -8584,7 +8593,7 @@
       <c r="J4" s="82"/>
       <c r="K4" s="82"/>
     </row>
-    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="96" t="s">
         <v>98</v>
       </c>
@@ -8613,7 +8622,7 @@
       <c r="J5" s="82"/>
       <c r="K5" s="82"/>
     </row>
-    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="96" t="s">
         <v>99</v>
       </c>
@@ -8642,7 +8651,7 @@
       <c r="J6" s="82"/>
       <c r="K6" s="82"/>
     </row>
-    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="96" t="s">
         <v>122</v>
       </c>
@@ -8663,7 +8672,7 @@
       <c r="J7" s="82"/>
       <c r="K7" s="82"/>
     </row>
-    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="96" t="s">
         <v>123</v>
       </c>
@@ -8684,7 +8693,7 @@
       <c r="J8" s="82"/>
       <c r="K8" s="82"/>
     </row>
-    <row r="9" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="96" t="s">
         <v>124</v>
       </c>
@@ -8705,7 +8714,7 @@
       <c r="J9" s="82"/>
       <c r="K9" s="82"/>
     </row>
-    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="96" t="s">
         <v>125</v>
       </c>
@@ -8726,7 +8735,7 @@
       <c r="J10" s="82"/>
       <c r="K10" s="82"/>
     </row>
-    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="96" t="s">
         <v>70</v>
       </c>
@@ -8747,7 +8756,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="96" t="s">
         <v>71</v>
       </c>
@@ -8766,7 +8775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="96" t="s">
         <v>72</v>
       </c>
@@ -8785,7 +8794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="96" t="s">
         <v>73</v>
       </c>
@@ -8805,7 +8814,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Y4zyQBYfuusMzk3xCuIBKA7S+ua9eXooxiuTcmsqRTtZ1YAFBCtzEh9wwodGgk5D9kCarW0M1B6RY/iOGTYjFQ==" saltValue="T0Qc6EKlR01WhM1CoiKT3A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="5SNpA1/HPzCbzlrUBzj8whfKZ4t3vdXeuP0XoS0SDZNp17FFywDOg8Z3QrtO/JYepe2FsA0lrJj3zdueIm2Tog==" saltValue="+/OKp618tncFKoeAhRnYjw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9795,7 +9804,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="cywgpVLfUgcqorNYzARrkMGX0uWLeKqyqf4XDB7IGthBtESQd440Hj4B8P1BMuSS9zUjnbHLRoDaT1G/v9tO7A==" saltValue="hKRxrjXSmV4HxmnMtEesIw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="59tgFZL193x7msuBksR8VoBDDceM0ljMEU97eRfuYyaaiUCxssW+dtJwfXgClynl6jaJEQjPfJ6uYWkIrUbtHQ==" saltValue="X9Cx/KZG2BxTpXQ8IlmqUw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="B2:I16 B18:I40 B17:C17 E17:I17">
     <cfRule type="expression" dxfId="0" priority="9">
       <formula>$A2=""</formula>
@@ -9856,7 +9865,7 @@
       <c r="A2" s="52" t="s">
         <v>232</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C2" s="96" t="s">
@@ -9878,8 +9887,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B3" s="107"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="108"/>
       <c r="C3" s="96" t="s">
         <v>154</v>
       </c>
@@ -9900,8 +9909,8 @@
       </c>
       <c r="J3" s="53"/>
     </row>
-    <row r="4" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B4" s="107"/>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="108"/>
       <c r="C4" s="96" t="s">
         <v>155</v>
       </c>
@@ -9922,8 +9931,8 @@
       </c>
       <c r="J4" s="53"/>
     </row>
-    <row r="5" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B5" s="106" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C5" s="96" t="s">
@@ -9946,8 +9955,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="107"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="108"/>
       <c r="C6" s="96" t="s">
         <v>154</v>
       </c>
@@ -9967,8 +9976,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="107"/>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="108"/>
       <c r="C7" s="96" t="s">
         <v>155</v>
       </c>
@@ -9988,8 +9997,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B8" s="106" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="107" t="s">
         <v>96</v>
       </c>
       <c r="C8" s="96" t="s">
@@ -10011,8 +10020,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="107"/>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="108"/>
       <c r="C9" s="96" t="s">
         <v>154</v>
       </c>
@@ -10032,8 +10041,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="107"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="108"/>
       <c r="C10" s="96" t="s">
         <v>155</v>
       </c>
@@ -10053,8 +10062,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B11" s="106" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="107" t="s">
         <v>97</v>
       </c>
       <c r="C11" s="96" t="s">
@@ -10076,8 +10085,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="107"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="108"/>
       <c r="C12" s="96" t="s">
         <v>154</v>
       </c>
@@ -10097,8 +10106,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B13" s="107"/>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="108"/>
       <c r="C13" s="96" t="s">
         <v>155</v>
       </c>
@@ -10118,8 +10127,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B14" s="106" t="s">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="107" t="s">
         <v>98</v>
       </c>
       <c r="C14" s="96" t="s">
@@ -10141,8 +10150,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="107"/>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="108"/>
       <c r="C15" s="96" t="s">
         <v>154</v>
       </c>
@@ -10162,8 +10171,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="107"/>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="108"/>
       <c r="C16" s="96" t="s">
         <v>155</v>
       </c>
@@ -10206,7 +10215,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D18" s="81"/>
       <c r="E18" s="81"/>
       <c r="F18" s="81"/>
@@ -10217,7 +10226,7 @@
       <c r="A19" s="52" t="s">
         <v>233</v>
       </c>
-      <c r="B19" s="106" t="s">
+      <c r="B19" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C19" s="96" t="s">
@@ -10239,8 +10248,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B20" s="107"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="108"/>
       <c r="C20" s="96" t="s">
         <v>154</v>
       </c>
@@ -10260,8 +10269,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="107"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="108"/>
       <c r="C21" s="96" t="s">
         <v>155</v>
       </c>
@@ -10281,8 +10290,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B22" s="106" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C22" s="96" t="s">
@@ -10304,8 +10313,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B23" s="107"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="108"/>
       <c r="C23" s="96" t="s">
         <v>154</v>
       </c>
@@ -10325,8 +10334,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B24" s="107"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="108"/>
       <c r="C24" s="96" t="s">
         <v>155</v>
       </c>
@@ -10346,8 +10355,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B25" s="106" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="107" t="s">
         <v>96</v>
       </c>
       <c r="C25" s="96" t="s">
@@ -10369,8 +10378,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="107"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="108"/>
       <c r="C26" s="96" t="s">
         <v>154</v>
       </c>
@@ -10390,8 +10399,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B27" s="107"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="108"/>
       <c r="C27" s="96" t="s">
         <v>155</v>
       </c>
@@ -10411,8 +10420,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B28" s="106" t="s">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="107" t="s">
         <v>97</v>
       </c>
       <c r="C28" s="96" t="s">
@@ -10434,8 +10443,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B29" s="107"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="108"/>
       <c r="C29" s="96" t="s">
         <v>154</v>
       </c>
@@ -10455,8 +10464,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B30" s="107"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="108"/>
       <c r="C30" s="96" t="s">
         <v>155</v>
       </c>
@@ -10476,8 +10485,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B31" s="106" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="107" t="s">
         <v>98</v>
       </c>
       <c r="C31" s="96" t="s">
@@ -10499,8 +10508,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B32" s="107"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="108"/>
       <c r="C32" s="96" t="s">
         <v>154</v>
       </c>
@@ -10520,8 +10529,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B33" s="107"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B33" s="108"/>
       <c r="C33" s="96" t="s">
         <v>155</v>
       </c>
@@ -10564,7 +10573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D35" s="81"/>
       <c r="E35" s="81"/>
       <c r="F35" s="81"/>
@@ -10575,7 +10584,7 @@
       <c r="A36" s="54" t="s">
         <v>234</v>
       </c>
-      <c r="B36" s="106" t="s">
+      <c r="B36" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C36" s="96" t="s">
@@ -10597,8 +10606,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B37" s="107"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="108"/>
       <c r="C37" s="96" t="s">
         <v>154</v>
       </c>
@@ -10618,8 +10627,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B38" s="107"/>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="108"/>
       <c r="C38" s="96" t="s">
         <v>155</v>
       </c>
@@ -10639,8 +10648,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B39" s="106" t="s">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C39" s="96" t="s">
@@ -10662,8 +10671,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B40" s="107"/>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B40" s="108"/>
       <c r="C40" s="96" t="s">
         <v>154</v>
       </c>
@@ -10683,8 +10692,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B41" s="107"/>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="108"/>
       <c r="C41" s="96" t="s">
         <v>155</v>
       </c>
@@ -10704,8 +10713,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B42" s="106" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="107" t="s">
         <v>96</v>
       </c>
       <c r="C42" s="96" t="s">
@@ -10727,8 +10736,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B43" s="107"/>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="108"/>
       <c r="C43" s="96" t="s">
         <v>154</v>
       </c>
@@ -10748,8 +10757,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B44" s="107"/>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="108"/>
       <c r="C44" s="96" t="s">
         <v>155</v>
       </c>
@@ -10769,8 +10778,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B45" s="106" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="107" t="s">
         <v>97</v>
       </c>
       <c r="C45" s="96" t="s">
@@ -10792,8 +10801,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B46" s="107"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B46" s="108"/>
       <c r="C46" s="96" t="s">
         <v>154</v>
       </c>
@@ -10813,8 +10822,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B47" s="107"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B47" s="108"/>
       <c r="C47" s="96" t="s">
         <v>155</v>
       </c>
@@ -10834,8 +10843,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B48" s="106" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B48" s="107" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="96" t="s">
@@ -10857,8 +10866,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B49" s="107"/>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="108"/>
       <c r="C49" s="96" t="s">
         <v>154</v>
       </c>
@@ -10878,8 +10887,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B50" s="107"/>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="108"/>
       <c r="C50" s="96" t="s">
         <v>155</v>
       </c>
@@ -10964,7 +10973,7 @@
       <c r="A55" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="B55" s="106" t="s">
+      <c r="B55" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C55" s="96" t="s">
@@ -10991,8 +11000,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B56" s="107"/>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="108"/>
       <c r="C56" s="96" t="s">
         <v>154</v>
       </c>
@@ -11017,8 +11026,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B57" s="107"/>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B57" s="108"/>
       <c r="C57" s="96" t="s">
         <v>155</v>
       </c>
@@ -11043,8 +11052,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B58" s="106" t="s">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C58" s="96" t="s">
@@ -11071,8 +11080,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B59" s="107"/>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="108"/>
       <c r="C59" s="96" t="s">
         <v>154</v>
       </c>
@@ -11097,8 +11106,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B60" s="107"/>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="108"/>
       <c r="C60" s="96" t="s">
         <v>155</v>
       </c>
@@ -11123,8 +11132,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B61" s="106" t="s">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="107" t="s">
         <v>96</v>
       </c>
       <c r="C61" s="96" t="s">
@@ -11151,8 +11160,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B62" s="107"/>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="108"/>
       <c r="C62" s="96" t="s">
         <v>154</v>
       </c>
@@ -11177,8 +11186,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B63" s="107"/>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="108"/>
       <c r="C63" s="96" t="s">
         <v>155</v>
       </c>
@@ -11203,8 +11212,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B64" s="106" t="s">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="107" t="s">
         <v>97</v>
       </c>
       <c r="C64" s="96" t="s">
@@ -11231,8 +11240,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B65" s="107"/>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B65" s="108"/>
       <c r="C65" s="96" t="s">
         <v>154</v>
       </c>
@@ -11257,8 +11266,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B66" s="107"/>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B66" s="108"/>
       <c r="C66" s="96" t="s">
         <v>155</v>
       </c>
@@ -11283,8 +11292,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B67" s="106" t="s">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B67" s="107" t="s">
         <v>98</v>
       </c>
       <c r="C67" s="96" t="s">
@@ -11311,8 +11320,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B68" s="107"/>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="108"/>
       <c r="C68" s="96" t="s">
         <v>154</v>
       </c>
@@ -11337,8 +11346,8 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
-      <c r="B69" s="107"/>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="108"/>
       <c r="C69" s="96" t="s">
         <v>155</v>
       </c>
@@ -11391,7 +11400,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D71" s="81"/>
       <c r="E71" s="81"/>
       <c r="F71" s="81"/>
@@ -11402,7 +11411,7 @@
       <c r="A72" s="52" t="s">
         <v>237</v>
       </c>
-      <c r="B72" s="106" t="s">
+      <c r="B72" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C72" s="96" t="s">
@@ -11430,7 +11439,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B73" s="107"/>
+      <c r="B73" s="108"/>
       <c r="C73" s="96" t="s">
         <v>154</v>
       </c>
@@ -11456,7 +11465,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="107"/>
+      <c r="B74" s="108"/>
       <c r="C74" s="96" t="s">
         <v>155</v>
       </c>
@@ -11482,7 +11491,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="106" t="s">
+      <c r="B75" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C75" s="96" t="s">
@@ -11510,7 +11519,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="107"/>
+      <c r="B76" s="108"/>
       <c r="C76" s="96" t="s">
         <v>154</v>
       </c>
@@ -11536,7 +11545,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="107"/>
+      <c r="B77" s="108"/>
       <c r="C77" s="96" t="s">
         <v>155</v>
       </c>
@@ -11562,7 +11571,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="106" t="s">
+      <c r="B78" s="107" t="s">
         <v>96</v>
       </c>
       <c r="C78" s="96" t="s">
@@ -11590,7 +11599,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="107"/>
+      <c r="B79" s="108"/>
       <c r="C79" s="96" t="s">
         <v>154</v>
       </c>
@@ -11616,7 +11625,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="107"/>
+      <c r="B80" s="108"/>
       <c r="C80" s="96" t="s">
         <v>155</v>
       </c>
@@ -11642,7 +11651,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="106" t="s">
+      <c r="B81" s="107" t="s">
         <v>97</v>
       </c>
       <c r="C81" s="96" t="s">
@@ -11670,7 +11679,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B82" s="107"/>
+      <c r="B82" s="108"/>
       <c r="C82" s="96" t="s">
         <v>154</v>
       </c>
@@ -11696,7 +11705,7 @@
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B83" s="107"/>
+      <c r="B83" s="108"/>
       <c r="C83" s="96" t="s">
         <v>155</v>
       </c>
@@ -11722,7 +11731,7 @@
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="106" t="s">
+      <c r="B84" s="107" t="s">
         <v>98</v>
       </c>
       <c r="C84" s="96" t="s">
@@ -11750,7 +11759,7 @@
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="107"/>
+      <c r="B85" s="108"/>
       <c r="C85" s="96" t="s">
         <v>154</v>
       </c>
@@ -11776,7 +11785,7 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B86" s="107"/>
+      <c r="B86" s="108"/>
       <c r="C86" s="96" t="s">
         <v>155</v>
       </c>
@@ -11840,7 +11849,7 @@
       <c r="A89" s="54" t="s">
         <v>238</v>
       </c>
-      <c r="B89" s="106" t="s">
+      <c r="B89" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C89" s="96" t="s">
@@ -11868,7 +11877,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B90" s="107"/>
+      <c r="B90" s="108"/>
       <c r="C90" s="96" t="s">
         <v>154</v>
       </c>
@@ -11894,7 +11903,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B91" s="107"/>
+      <c r="B91" s="108"/>
       <c r="C91" s="96" t="s">
         <v>155</v>
       </c>
@@ -11920,7 +11929,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B92" s="106" t="s">
+      <c r="B92" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C92" s="96" t="s">
@@ -11948,7 +11957,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B93" s="107"/>
+      <c r="B93" s="108"/>
       <c r="C93" s="96" t="s">
         <v>154</v>
       </c>
@@ -11974,7 +11983,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B94" s="107"/>
+      <c r="B94" s="108"/>
       <c r="C94" s="96" t="s">
         <v>155</v>
       </c>
@@ -12000,7 +12009,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B95" s="106" t="s">
+      <c r="B95" s="107" t="s">
         <v>96</v>
       </c>
       <c r="C95" s="96" t="s">
@@ -12028,7 +12037,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="107"/>
+      <c r="B96" s="108"/>
       <c r="C96" s="96" t="s">
         <v>154</v>
       </c>
@@ -12054,7 +12063,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="107"/>
+      <c r="B97" s="108"/>
       <c r="C97" s="96" t="s">
         <v>155</v>
       </c>
@@ -12080,7 +12089,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B98" s="106" t="s">
+      <c r="B98" s="107" t="s">
         <v>97</v>
       </c>
       <c r="C98" s="96" t="s">
@@ -12108,7 +12117,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B99" s="107"/>
+      <c r="B99" s="108"/>
       <c r="C99" s="96" t="s">
         <v>154</v>
       </c>
@@ -12134,7 +12143,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B100" s="107"/>
+      <c r="B100" s="108"/>
       <c r="C100" s="96" t="s">
         <v>155</v>
       </c>
@@ -12160,7 +12169,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B101" s="106" t="s">
+      <c r="B101" s="107" t="s">
         <v>98</v>
       </c>
       <c r="C101" s="96" t="s">
@@ -12188,7 +12197,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B102" s="107"/>
+      <c r="B102" s="108"/>
       <c r="C102" s="96" t="s">
         <v>154</v>
       </c>
@@ -12214,7 +12223,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B103" s="107"/>
+      <c r="B103" s="108"/>
       <c r="C103" s="96" t="s">
         <v>155</v>
       </c>
@@ -12309,7 +12318,7 @@
       <c r="A108" s="52" t="s">
         <v>240</v>
       </c>
-      <c r="B108" s="106" t="s">
+      <c r="B108" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C108" s="96" t="s">
@@ -12337,7 +12346,7 @@
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B109" s="107"/>
+      <c r="B109" s="108"/>
       <c r="C109" s="96" t="s">
         <v>154</v>
       </c>
@@ -12363,7 +12372,7 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B110" s="107"/>
+      <c r="B110" s="108"/>
       <c r="C110" s="96" t="s">
         <v>155</v>
       </c>
@@ -12389,7 +12398,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B111" s="106" t="s">
+      <c r="B111" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C111" s="96" t="s">
@@ -12417,7 +12426,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B112" s="107"/>
+      <c r="B112" s="108"/>
       <c r="C112" s="96" t="s">
         <v>154</v>
       </c>
@@ -12443,7 +12452,7 @@
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B113" s="107"/>
+      <c r="B113" s="108"/>
       <c r="C113" s="96" t="s">
         <v>155</v>
       </c>
@@ -12469,7 +12478,7 @@
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B114" s="106" t="s">
+      <c r="B114" s="107" t="s">
         <v>96</v>
       </c>
       <c r="C114" s="96" t="s">
@@ -12497,7 +12506,7 @@
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B115" s="107"/>
+      <c r="B115" s="108"/>
       <c r="C115" s="96" t="s">
         <v>154</v>
       </c>
@@ -12523,7 +12532,7 @@
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B116" s="107"/>
+      <c r="B116" s="108"/>
       <c r="C116" s="96" t="s">
         <v>155</v>
       </c>
@@ -12549,7 +12558,7 @@
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B117" s="106" t="s">
+      <c r="B117" s="107" t="s">
         <v>97</v>
       </c>
       <c r="C117" s="96" t="s">
@@ -12577,7 +12586,7 @@
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B118" s="107"/>
+      <c r="B118" s="108"/>
       <c r="C118" s="96" t="s">
         <v>154</v>
       </c>
@@ -12603,7 +12612,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B119" s="107"/>
+      <c r="B119" s="108"/>
       <c r="C119" s="96" t="s">
         <v>155</v>
       </c>
@@ -12629,7 +12638,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B120" s="106" t="s">
+      <c r="B120" s="107" t="s">
         <v>98</v>
       </c>
       <c r="C120" s="96" t="s">
@@ -12657,7 +12666,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B121" s="107"/>
+      <c r="B121" s="108"/>
       <c r="C121" s="96" t="s">
         <v>154</v>
       </c>
@@ -12683,7 +12692,7 @@
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B122" s="107"/>
+      <c r="B122" s="108"/>
       <c r="C122" s="96" t="s">
         <v>155</v>
       </c>
@@ -12747,7 +12756,7 @@
       <c r="A125" s="52" t="s">
         <v>241</v>
       </c>
-      <c r="B125" s="106" t="s">
+      <c r="B125" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C125" s="96" t="s">
@@ -12775,7 +12784,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B126" s="107"/>
+      <c r="B126" s="108"/>
       <c r="C126" s="96" t="s">
         <v>154</v>
       </c>
@@ -12801,7 +12810,7 @@
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B127" s="107"/>
+      <c r="B127" s="108"/>
       <c r="C127" s="96" t="s">
         <v>155</v>
       </c>
@@ -12827,7 +12836,7 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B128" s="106" t="s">
+      <c r="B128" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C128" s="96" t="s">
@@ -12855,7 +12864,7 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B129" s="107"/>
+      <c r="B129" s="108"/>
       <c r="C129" s="96" t="s">
         <v>154</v>
       </c>
@@ -12881,7 +12890,7 @@
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B130" s="107"/>
+      <c r="B130" s="108"/>
       <c r="C130" s="96" t="s">
         <v>155</v>
       </c>
@@ -12907,7 +12916,7 @@
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B131" s="106" t="s">
+      <c r="B131" s="107" t="s">
         <v>96</v>
       </c>
       <c r="C131" s="96" t="s">
@@ -12935,7 +12944,7 @@
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B132" s="107"/>
+      <c r="B132" s="108"/>
       <c r="C132" s="96" t="s">
         <v>154</v>
       </c>
@@ -12961,7 +12970,7 @@
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B133" s="107"/>
+      <c r="B133" s="108"/>
       <c r="C133" s="96" t="s">
         <v>155</v>
       </c>
@@ -12987,7 +12996,7 @@
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B134" s="106" t="s">
+      <c r="B134" s="107" t="s">
         <v>97</v>
       </c>
       <c r="C134" s="96" t="s">
@@ -13015,7 +13024,7 @@
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B135" s="107"/>
+      <c r="B135" s="108"/>
       <c r="C135" s="96" t="s">
         <v>154</v>
       </c>
@@ -13041,7 +13050,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B136" s="107"/>
+      <c r="B136" s="108"/>
       <c r="C136" s="96" t="s">
         <v>155</v>
       </c>
@@ -13067,7 +13076,7 @@
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B137" s="106" t="s">
+      <c r="B137" s="107" t="s">
         <v>98</v>
       </c>
       <c r="C137" s="96" t="s">
@@ -13095,7 +13104,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B138" s="107"/>
+      <c r="B138" s="108"/>
       <c r="C138" s="96" t="s">
         <v>154</v>
       </c>
@@ -13121,7 +13130,7 @@
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B139" s="107"/>
+      <c r="B139" s="108"/>
       <c r="C139" s="96" t="s">
         <v>155</v>
       </c>
@@ -13185,7 +13194,7 @@
       <c r="A142" s="54" t="s">
         <v>242</v>
       </c>
-      <c r="B142" s="106" t="s">
+      <c r="B142" s="107" t="s">
         <v>100</v>
       </c>
       <c r="C142" s="96" t="s">
@@ -13213,7 +13222,7 @@
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B143" s="107"/>
+      <c r="B143" s="108"/>
       <c r="C143" s="96" t="s">
         <v>154</v>
       </c>
@@ -13239,7 +13248,7 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B144" s="107"/>
+      <c r="B144" s="108"/>
       <c r="C144" s="96" t="s">
         <v>155</v>
       </c>
@@ -13265,7 +13274,7 @@
       </c>
     </row>
     <row r="145" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B145" s="106" t="s">
+      <c r="B145" s="107" t="s">
         <v>109</v>
       </c>
       <c r="C145" s="96" t="s">
@@ -13293,7 +13302,7 @@
       </c>
     </row>
     <row r="146" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B146" s="107"/>
+      <c r="B146" s="108"/>
       <c r="C146" s="96" t="s">
         <v>154</v>
       </c>
@@ -13319,7 +13328,7 @@
       </c>
     </row>
     <row r="147" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B147" s="107"/>
+      <c r="B147" s="108"/>
       <c r="C147" s="96" t="s">
         <v>155</v>
       </c>
@@ -13345,7 +13354,7 @@
       </c>
     </row>
     <row r="148" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B148" s="106" t="s">
+      <c r="B148" s="107" t="s">
         <v>96</v>
       </c>
       <c r="C148" s="96" t="s">
@@ -13373,7 +13382,7 @@
       </c>
     </row>
     <row r="149" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B149" s="107"/>
+      <c r="B149" s="108"/>
       <c r="C149" s="96" t="s">
         <v>154</v>
       </c>
@@ -13399,7 +13408,7 @@
       </c>
     </row>
     <row r="150" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B150" s="107"/>
+      <c r="B150" s="108"/>
       <c r="C150" s="96" t="s">
         <v>155</v>
       </c>
@@ -13425,7 +13434,7 @@
       </c>
     </row>
     <row r="151" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B151" s="106" t="s">
+      <c r="B151" s="107" t="s">
         <v>97</v>
       </c>
       <c r="C151" s="96" t="s">
@@ -13453,7 +13462,7 @@
       </c>
     </row>
     <row r="152" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B152" s="107"/>
+      <c r="B152" s="108"/>
       <c r="C152" s="96" t="s">
         <v>154</v>
       </c>
@@ -13479,7 +13488,7 @@
       </c>
     </row>
     <row r="153" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B153" s="107"/>
+      <c r="B153" s="108"/>
       <c r="C153" s="96" t="s">
         <v>155</v>
       </c>
@@ -13505,7 +13514,7 @@
       </c>
     </row>
     <row r="154" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B154" s="106" t="s">
+      <c r="B154" s="107" t="s">
         <v>98</v>
       </c>
       <c r="C154" s="96" t="s">
@@ -13533,7 +13542,7 @@
       </c>
     </row>
     <row r="155" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B155" s="107"/>
+      <c r="B155" s="108"/>
       <c r="C155" s="96" t="s">
         <v>154</v>
       </c>
@@ -13559,7 +13568,7 @@
       </c>
     </row>
     <row r="156" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B156" s="107"/>
+      <c r="B156" s="108"/>
       <c r="C156" s="96" t="s">
         <v>155</v>
       </c>
@@ -13613,8 +13622,44 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="1E74N2mLrkaxzGPm3U5JnA1MstNuTIb3HiT8l7zSWKd4x3+3bigpVsjAlt/bW/+eR8oaRtxfjbCBti61ptohoA==" saltValue="CecqxznHFh1jvEivzLZGvA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="RTr4YZRu8YgEhwPv+AHrSbFfDBSY4RyMZjpGsfANknFZnbqk8IoT2YkbMvh96sgywM/9htRw6ycs96Ng0+qUwg==" saltValue="wGHiKLNQ4tNRiisLHkSyaw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="45">
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B58:B60"/>
+    <mergeCell ref="B61:B63"/>
+    <mergeCell ref="B64:B66"/>
+    <mergeCell ref="B67:B69"/>
+    <mergeCell ref="B72:B74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="B81:B83"/>
+    <mergeCell ref="B84:B86"/>
+    <mergeCell ref="B108:B110"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="B92:B94"/>
+    <mergeCell ref="B95:B97"/>
+    <mergeCell ref="B98:B100"/>
+    <mergeCell ref="B101:B103"/>
+    <mergeCell ref="B111:B113"/>
+    <mergeCell ref="B114:B116"/>
+    <mergeCell ref="B117:B119"/>
+    <mergeCell ref="B120:B122"/>
+    <mergeCell ref="B125:B127"/>
     <mergeCell ref="B145:B147"/>
     <mergeCell ref="B148:B150"/>
     <mergeCell ref="B151:B153"/>
@@ -13624,42 +13669,6 @@
     <mergeCell ref="B134:B136"/>
     <mergeCell ref="B137:B139"/>
     <mergeCell ref="B142:B144"/>
-    <mergeCell ref="B111:B113"/>
-    <mergeCell ref="B114:B116"/>
-    <mergeCell ref="B117:B119"/>
-    <mergeCell ref="B120:B122"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="B108:B110"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="B92:B94"/>
-    <mergeCell ref="B95:B97"/>
-    <mergeCell ref="B98:B100"/>
-    <mergeCell ref="B101:B103"/>
-    <mergeCell ref="B72:B74"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="B81:B83"/>
-    <mergeCell ref="B84:B86"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B58:B60"/>
-    <mergeCell ref="B61:B63"/>
-    <mergeCell ref="B64:B66"/>
-    <mergeCell ref="B67:B69"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="B25:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B33"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -14880,7 +14889,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="wBqWqNVLf6fThieJFIpKhEaBMMg00uWBYR001c7Aj1CCEPHrxwaQFrknwLInCWA9pivPbVVkZG3u2OvN7m/UWA==" saltValue="WmHblSPQ4wYwzvFo36eZ9g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="73L0fVO8LMo+kDtmJhCju+UvrRENvcMghbtG2DIDoYoUueGHh3fnDbQJi93zW/L+JF+NeqcCLX2VRrj6zAPLZQ==" saltValue="D65V9WpNDEG+yFkenC+9xg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -21052,7 +21061,7 @@
       <c r="H248" s="64"/>
       <c r="I248" s="64"/>
     </row>
-    <row r="249" spans="1:9" ht="26" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:9" ht="13" x14ac:dyDescent="0.3">
       <c r="A249" s="72" t="s">
         <v>279</v>
       </c>
@@ -23019,7 +23028,7 @@
       <c r="I328" s="72"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="NdHvzRFNumjXQd7J6esWVmzGgjWLTLsZmvJwShYaA31riq9wDUJzt1Wn2CVH3edLTFbef3ILrt6bcSh4YsgtNQ==" saltValue="xL+3zH8aK2570+sWrgTGyA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="dGG8XXi7a+jL4CoFf/FukHStbtAQ5tz+hS1o5HZEed6GAwWJuE/GjC3rEDInTRD3DQe3jqnF+oAnKPtKDhSv5w==" saltValue="SK0Xtc8MCMxxAk6I1mdbVg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -24109,7 +24118,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KCtM1I/IApQ4tUIC2REHyarifoxeoaq50eakqeu16Ebkf3gLCf9mTboYsLX3T0OnhuJ2FXmZ3PrWkAzS2uOz9w==" saltValue="+jrVtQtSJngm1RTHr6v7lw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="94d3F9twXAARU74Ouuuh8fEcC6eZgpkUZp687NJ38x2YVhL2dE2zBZdCmodoJstZgJwIBrOe9DMBftEtpjmIQQ==" saltValue="c/a7gIaGENrGAw+CEemeYA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -24981,7 +24990,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="4nIb5ilgK2YX9To+A4XGMXnm56LR9bwtd/bWkzKkp1fw5AAeE70NGh0AVFadrjwxZmgXR8TVOJWcT4ErDLURIA==" saltValue="ftjvIj46nU1rrdh1RKzh5Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="q8XKjg5CQxyChNG9SjU60kVeTRx2UYBbhiLJlXZtfHq+DNvg+6dM4y6161arbLjO1ms61KPKYxq/P1dNI5kYPA==" saltValue="9IdfLMP8UyssZTYZWsiJyQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -27866,7 +27875,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="vUv1ZHGVOdUAhFvas1zyzRXBTqDVfTt/UxzqNcMFtGrf5vjrwR+Be1+Yup9NwsG1DxuzPAYVVchhDlxIjH4N5Q==" saltValue="LbFcqCh8xWiOveS5rUNanA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="0ZkIG0xXH27VS56XXDI7tKEqXHOUT4KGKqx85Syc8w7Kgfsi7Xl2kpCXOqylV2yUF9V9Q/WY4UMm/95NitvrDQ==" saltValue="rejMo134z258eD+42WlarA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -27916,7 +27925,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="65" t="s">
         <v>161</v>
       </c>
@@ -27947,7 +27956,7 @@
       <c r="F4" s="77"/>
       <c r="G4" s="77"/>
     </row>
-    <row r="5" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="69" t="s">
         <v>165</v>
       </c>
@@ -27996,7 +28005,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="65" t="s">
         <v>161</v>
       </c>
@@ -28032,7 +28041,7 @@
       <c r="F11" s="77"/>
       <c r="G11" s="77"/>
     </row>
-    <row r="12" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" s="69" t="s">
         <v>165</v>
       </c>
@@ -28086,7 +28095,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="65" t="s">
         <v>161</v>
       </c>
@@ -28122,7 +28131,7 @@
       <c r="F18" s="77"/>
       <c r="G18" s="77"/>
     </row>
-    <row r="19" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" s="69" t="s">
         <v>165</v>
       </c>
@@ -28148,7 +28157,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="b/dMJqg/oFWrZE2sWbZM3eP0UtSiP9UKY41D0m7OlktYxINy2pA1mm44jPrg7nbbwSpPzBlWlrh2gWCPdy/yeA==" saltValue="Q4JCMuoZGxDCz1oXAGhAVw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="79hDzam5WrL+oEjr5RoCdypb/zTML8BczRMNPRyYMX0yM2Ea7KKOGGuZHRW9CtkihZvBEMo5zmsY9K/kEpcgRA==" saltValue="03OiLDi5JhJXmtLK47QmoQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -28205,7 +28214,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="69" t="s">
         <v>193</v>
       </c>
@@ -28231,7 +28240,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="69" t="s">
         <v>333</v>
       </c>
@@ -28251,7 +28260,7 @@
         <v>0.53134328358208949</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="69" t="s">
         <v>334</v>
       </c>
@@ -28271,7 +28280,7 @@
         <v>0.38507462686567179</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
         <v>192</v>
       </c>
@@ -28297,7 +28306,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="69" t="s">
         <v>334</v>
       </c>
@@ -28317,7 +28326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="69" t="s">
         <v>209</v>
       </c>
@@ -28340,7 +28349,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="69" t="s">
         <v>334</v>
       </c>
@@ -28360,7 +28369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="69" t="s">
         <v>185</v>
       </c>
@@ -28386,7 +28395,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="69" t="s">
         <v>334</v>
       </c>
@@ -28406,7 +28415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="69" t="s">
         <v>209</v>
       </c>
@@ -28429,7 +28438,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" s="69" t="s">
         <v>334</v>
       </c>
@@ -28449,7 +28458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="69" t="s">
         <v>205</v>
       </c>
@@ -28475,7 +28484,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="69" t="s">
         <v>334</v>
       </c>
@@ -28495,7 +28504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="69" t="s">
         <v>209</v>
       </c>
@@ -28518,7 +28527,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="69" t="s">
         <v>334</v>
       </c>
@@ -28538,7 +28547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="69" t="s">
         <v>170</v>
       </c>
@@ -28564,7 +28573,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C18" s="69" t="s">
         <v>334</v>
       </c>
@@ -28584,7 +28593,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="69" t="s">
         <v>209</v>
       </c>
@@ -28607,7 +28616,7 @@
         <v>0.33500000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C20" s="69" t="s">
         <v>334</v>
       </c>
@@ -28627,7 +28636,7 @@
         <v>0.62</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="69" t="s">
         <v>175</v>
       </c>
@@ -28653,7 +28662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C22" s="69" t="s">
         <v>333</v>
       </c>
@@ -28673,7 +28682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="69" t="s">
         <v>173</v>
       </c>
@@ -28699,7 +28708,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C24" s="69" t="s">
         <v>333</v>
       </c>
@@ -28719,7 +28728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="69" t="s">
         <v>174</v>
       </c>
@@ -28745,7 +28754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C26" s="69" t="s">
         <v>333</v>
       </c>
@@ -28765,7 +28774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="69" t="s">
         <v>197</v>
       </c>
@@ -28791,7 +28800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C28" s="69" t="s">
         <v>333</v>
       </c>
@@ -28811,7 +28820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C29" s="69" t="s">
         <v>334</v>
       </c>
@@ -28831,7 +28840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="69" t="s">
         <v>198</v>
       </c>
@@ -28857,7 +28866,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C31" s="69" t="s">
         <v>333</v>
       </c>
@@ -28877,7 +28886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C32" s="69" t="s">
         <v>334</v>
       </c>
@@ -28897,7 +28906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="69" t="s">
         <v>196</v>
       </c>
@@ -28923,7 +28932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C34" s="69" t="s">
         <v>333</v>
       </c>
@@ -28943,7 +28952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C35" s="69" t="s">
         <v>334</v>
       </c>
@@ -28963,7 +28972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="69" t="s">
         <v>195</v>
       </c>
@@ -28989,7 +28998,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C37" s="69" t="s">
         <v>333</v>
       </c>
@@ -29009,7 +29018,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C38" s="69" t="s">
         <v>334</v>
       </c>
@@ -29029,7 +29038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="69" t="s">
         <v>194</v>
       </c>
@@ -29055,7 +29064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C40" s="69" t="s">
         <v>333</v>
       </c>
@@ -29075,7 +29084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C41" s="69" t="s">
         <v>334</v>
       </c>
@@ -29095,7 +29104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="69" t="s">
         <v>200</v>
       </c>
@@ -29121,7 +29130,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C43" s="69" t="s">
         <v>333</v>
       </c>
@@ -29141,7 +29150,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C44" s="69" t="s">
         <v>334</v>
       </c>
@@ -29161,7 +29170,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B45" s="69" t="s">
         <v>88</v>
       </c>
@@ -29184,7 +29193,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C46" s="69" t="s">
         <v>333</v>
       </c>
@@ -29204,7 +29213,7 @@
         <v>0.49</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C47" s="69" t="s">
         <v>334</v>
       </c>
@@ -29224,7 +29233,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="69" t="s">
         <v>191</v>
       </c>
@@ -29250,7 +29259,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C49" s="69" t="s">
         <v>333</v>
       </c>
@@ -29270,7 +29279,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="69" t="s">
         <v>199</v>
       </c>
@@ -29296,7 +29305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C51" s="69" t="s">
         <v>333</v>
       </c>
@@ -29316,7 +29325,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="69" t="s">
         <v>184</v>
       </c>
@@ -29342,7 +29351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C53" s="69" t="s">
         <v>333</v>
       </c>
@@ -29395,7 +29404,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="69" t="s">
         <v>193</v>
       </c>
@@ -29426,7 +29435,7 @@
         <v>0.30150000000000005</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C58" s="69" t="s">
         <v>333</v>
       </c>
@@ -29451,7 +29460,7 @@
         <v>0.47820895522388057</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C59" s="69" t="s">
         <v>334</v>
       </c>
@@ -29476,7 +29485,7 @@
         <v>0.3465671641791046</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="69" t="s">
         <v>192</v>
       </c>
@@ -29507,7 +29516,7 @@
         <v>0.30150000000000005</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C61" s="69" t="s">
         <v>334</v>
       </c>
@@ -29532,7 +29541,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B62" s="69" t="s">
         <v>209</v>
       </c>
@@ -29560,7 +29569,7 @@
         <v>0.30150000000000005</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C63" s="69" t="s">
         <v>334</v>
       </c>
@@ -29585,7 +29594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="69" t="s">
         <v>185</v>
       </c>
@@ -29616,7 +29625,7 @@
         <v>0.30150000000000005</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C65" s="69" t="s">
         <v>334</v>
       </c>
@@ -29641,7 +29650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B66" s="69" t="s">
         <v>209</v>
       </c>
@@ -29669,7 +29678,7 @@
         <v>0.30150000000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C67" s="69" t="s">
         <v>334</v>
       </c>
@@ -29694,7 +29703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="69" t="s">
         <v>205</v>
       </c>
@@ -29725,7 +29734,7 @@
         <v>0.30150000000000005</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C69" s="69" t="s">
         <v>334</v>
       </c>
@@ -29750,7 +29759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B70" s="69" t="s">
         <v>209</v>
       </c>
@@ -29778,7 +29787,7 @@
         <v>0.30150000000000005</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C71" s="69" t="s">
         <v>334</v>
       </c>
@@ -29803,7 +29812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="69" t="s">
         <v>170</v>
       </c>
@@ -29834,7 +29843,7 @@
         <v>0.30150000000000005</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C73" s="69" t="s">
         <v>334</v>
       </c>
@@ -29859,7 +29868,7 @@
         <v>0.55800000000000005</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B74" s="69" t="s">
         <v>209</v>
       </c>
@@ -29887,7 +29896,7 @@
         <v>0.30150000000000005</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C75" s="69" t="s">
         <v>334</v>
       </c>
@@ -29912,7 +29921,7 @@
         <v>0.55800000000000005</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="69" t="s">
         <v>175</v>
       </c>
@@ -29943,7 +29952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C77" s="69" t="s">
         <v>333</v>
       </c>
@@ -29968,7 +29977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="69" t="s">
         <v>173</v>
       </c>
@@ -29999,7 +30008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C79" s="69" t="s">
         <v>333</v>
       </c>
@@ -30024,7 +30033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="69" t="s">
         <v>174</v>
       </c>
@@ -30055,7 +30064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C81" s="69" t="s">
         <v>333</v>
       </c>
@@ -30080,7 +30089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="69" t="s">
         <v>197</v>
       </c>
@@ -30111,7 +30120,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C83" s="69" t="s">
         <v>333</v>
       </c>
@@ -30136,7 +30145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C84" s="69" t="s">
         <v>334</v>
       </c>
@@ -30161,7 +30170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="69" t="s">
         <v>198</v>
       </c>
@@ -30192,7 +30201,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C86" s="69" t="s">
         <v>333</v>
       </c>
@@ -30217,7 +30226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C87" s="69" t="s">
         <v>334</v>
       </c>
@@ -30242,7 +30251,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="69" t="s">
         <v>196</v>
       </c>
@@ -30273,7 +30282,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C89" s="69" t="s">
         <v>333</v>
       </c>
@@ -30298,7 +30307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C90" s="69" t="s">
         <v>334</v>
       </c>
@@ -30323,7 +30332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="69" t="s">
         <v>195</v>
       </c>
@@ -30354,7 +30363,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C92" s="69" t="s">
         <v>333</v>
       </c>
@@ -30379,7 +30388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C93" s="69" t="s">
         <v>334</v>
       </c>
@@ -30404,7 +30413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="69" t="s">
         <v>194</v>
       </c>
@@ -30435,7 +30444,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C95" s="69" t="s">
         <v>333</v>
       </c>
@@ -30460,7 +30469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C96" s="69" t="s">
         <v>334</v>
       </c>
@@ -30485,7 +30494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="69" t="s">
         <v>200</v>
       </c>
@@ -30516,7 +30525,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C98" s="69" t="s">
         <v>333</v>
       </c>
@@ -30541,7 +30550,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C99" s="69" t="s">
         <v>334</v>
       </c>
@@ -30566,7 +30575,7 @@
         <v>0.58500000000000008</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B100" s="69" t="s">
         <v>88</v>
       </c>
@@ -30594,7 +30603,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C101" s="69" t="s">
         <v>333</v>
       </c>
@@ -30619,7 +30628,7 @@
         <v>0.441</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C102" s="69" t="s">
         <v>334</v>
       </c>
@@ -30644,7 +30653,7 @@
         <v>0.46800000000000003</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="69" t="s">
         <v>191</v>
       </c>
@@ -30675,7 +30684,7 @@
         <v>0.79200000000000004</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C104" s="69" t="s">
         <v>333</v>
       </c>
@@ -30700,7 +30709,7 @@
         <v>0.83700000000000008</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="69" t="s">
         <v>199</v>
       </c>
@@ -30731,7 +30740,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C106" s="69" t="s">
         <v>333</v>
       </c>
@@ -30756,7 +30765,7 @@
         <v>0.77400000000000002</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="69" t="s">
         <v>184</v>
       </c>
@@ -30787,7 +30796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C108" s="69" t="s">
         <v>333</v>
       </c>
@@ -30845,7 +30854,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="69" t="s">
         <v>193</v>
       </c>
@@ -30876,7 +30885,7 @@
         <v>0.35175000000000006</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C113" s="69" t="s">
         <v>333</v>
       </c>
@@ -30901,7 +30910,7 @@
         <v>0.55791044776119403</v>
       </c>
     </row>
-    <row r="114" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C114" s="69" t="s">
         <v>334</v>
       </c>
@@ -30926,7 +30935,7 @@
         <v>0.40432835820895541</v>
       </c>
     </row>
-    <row r="115" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="69" t="s">
         <v>192</v>
       </c>
@@ -30957,7 +30966,7 @@
         <v>0.35175000000000006</v>
       </c>
     </row>
-    <row r="116" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C116" s="69" t="s">
         <v>334</v>
       </c>
@@ -30982,7 +30991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B117" s="69" t="s">
         <v>209</v>
       </c>
@@ -31010,7 +31019,7 @@
         <v>0.35175000000000006</v>
       </c>
     </row>
-    <row r="118" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C118" s="69" t="s">
         <v>334</v>
       </c>
@@ -31035,7 +31044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="69" t="s">
         <v>185</v>
       </c>
@@ -31066,7 +31075,7 @@
         <v>0.35175000000000006</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C120" s="69" t="s">
         <v>334</v>
       </c>
@@ -31091,7 +31100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B121" s="69" t="s">
         <v>209</v>
       </c>
@@ -31119,7 +31128,7 @@
         <v>0.35175000000000006</v>
       </c>
     </row>
-    <row r="122" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C122" s="69" t="s">
         <v>334</v>
       </c>
@@ -31144,7 +31153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="69" t="s">
         <v>205</v>
       </c>
@@ -31175,7 +31184,7 @@
         <v>0.35175000000000006</v>
       </c>
     </row>
-    <row r="124" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C124" s="69" t="s">
         <v>334</v>
       </c>
@@ -31200,7 +31209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B125" s="69" t="s">
         <v>209</v>
       </c>
@@ -31228,7 +31237,7 @@
         <v>0.35175000000000006</v>
       </c>
     </row>
-    <row r="126" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C126" s="69" t="s">
         <v>334</v>
       </c>
@@ -31253,7 +31262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="69" t="s">
         <v>170</v>
       </c>
@@ -31284,7 +31293,7 @@
         <v>0.35175000000000006</v>
       </c>
     </row>
-    <row r="128" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C128" s="69" t="s">
         <v>334</v>
       </c>
@@ -31309,7 +31318,7 @@
         <v>0.65100000000000002</v>
       </c>
     </row>
-    <row r="129" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B129" s="69" t="s">
         <v>209</v>
       </c>
@@ -31337,7 +31346,7 @@
         <v>0.35175000000000006</v>
       </c>
     </row>
-    <row r="130" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C130" s="69" t="s">
         <v>334</v>
       </c>
@@ -31362,7 +31371,7 @@
         <v>0.65100000000000002</v>
       </c>
     </row>
-    <row r="131" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="69" t="s">
         <v>175</v>
       </c>
@@ -31393,7 +31402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C132" s="69" t="s">
         <v>333</v>
       </c>
@@ -31418,7 +31427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="69" t="s">
         <v>173</v>
       </c>
@@ -31449,7 +31458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C134" s="69" t="s">
         <v>333</v>
       </c>
@@ -31474,7 +31483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="69" t="s">
         <v>174</v>
       </c>
@@ -31505,7 +31514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C136" s="69" t="s">
         <v>333</v>
       </c>
@@ -31530,7 +31539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="69" t="s">
         <v>197</v>
       </c>
@@ -31561,7 +31570,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="138" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C138" s="69" t="s">
         <v>333</v>
       </c>
@@ -31586,7 +31595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C139" s="69" t="s">
         <v>334</v>
       </c>
@@ -31611,7 +31620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="69" t="s">
         <v>198</v>
       </c>
@@ -32263,7 +32272,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Wzqq08/t9kc16MupN5jONBuNJFGI++vrvcPgssVhffDGy9QrGnLxbhmdcr7i87x2AkLDciBgBOG7ePnW+KynJQ==" saltValue="sqjqMCfYr5xtduMjHmhtaQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Vc3h5nfsJK7iKj49GvDqPkcO6snZ2y/0hmiXrz/+9w3374wL+zU3/rVLwkzcpJ60HMtYAkmmBNM7lBXhlqJ/eA==" saltValue="pb1HI+/ZQEE9+vi6WEG+vw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -32312,7 +32321,7 @@
       </c>
       <c r="H1" s="52"/>
     </row>
-    <row r="2" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="78" t="s">
         <v>169</v>
       </c>
@@ -32336,7 +32345,7 @@
       </c>
       <c r="H2" s="69"/>
     </row>
-    <row r="3" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="96" t="s">
         <v>333</v>
       </c>
@@ -32354,7 +32363,7 @@
       </c>
       <c r="H3" s="78"/>
     </row>
-    <row r="4" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="78" t="s">
         <v>188</v>
       </c>
@@ -32378,7 +32387,7 @@
       </c>
       <c r="H4" s="78"/>
     </row>
-    <row r="5" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="96" t="s">
         <v>333</v>
       </c>
@@ -32396,7 +32405,7 @@
       </c>
       <c r="H5" s="69"/>
     </row>
-    <row r="6" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="78" t="s">
         <v>187</v>
       </c>
@@ -32420,7 +32429,7 @@
       </c>
       <c r="H6" s="69"/>
     </row>
-    <row r="7" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="96" t="s">
         <v>333</v>
       </c>
@@ -32464,7 +32473,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="78" t="s">
         <v>169</v>
       </c>
@@ -32491,7 +32500,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" s="96" t="s">
         <v>333</v>
       </c>
@@ -32512,7 +32521,7 @@
         <v>0.18000000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="78" t="s">
         <v>188</v>
       </c>
@@ -32539,7 +32548,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" s="96" t="s">
         <v>333</v>
       </c>
@@ -32560,7 +32569,7 @@
         <v>0.53100000000000003</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="78" t="s">
         <v>187</v>
       </c>
@@ -32587,7 +32596,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" s="96" t="s">
         <v>333</v>
       </c>
@@ -32634,7 +32643,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="78" t="s">
         <v>169</v>
       </c>
@@ -32661,7 +32670,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C21" s="96" t="s">
         <v>333</v>
       </c>
@@ -32682,7 +32691,7 @@
         <v>0.21000000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="78" t="s">
         <v>188</v>
       </c>
@@ -32709,7 +32718,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C23" s="96" t="s">
         <v>333</v>
       </c>
@@ -32730,7 +32739,7 @@
         <v>0.61949999999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="78" t="s">
         <v>187</v>
       </c>
@@ -32757,7 +32766,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C25" s="96" t="s">
         <v>333</v>
       </c>
@@ -32779,7 +32788,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="VJwY6wLu21gQCiPHUvseQig9p1EJh/+41DaLwFcJzgcjRrBokjMCuq0McI5rec09TtAQBkJU2mgFOKheuRWngw==" saltValue="E4QWPKLlYwnXmToG+dK1xA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="C81VN1Mc5RLvIRGWFGIm1pzzxDAMBVfb7WYh+/stGexEzTwMsu/gsOFGKIboSEX4YpLXnfvLcARoIns1yxXt1A==" saltValue="elbTiNfSG9apWmhzoT5lzA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -32792,7 +32801,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C11" activeCellId="2" sqref="C35 C23:F23 C11"/>
+      <selection activeCell="C13" sqref="C13:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -32903,16 +32912,16 @@
       <c r="B13" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="106" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="106" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="106" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="106" t="s">
         <v>99</v>
       </c>
       <c r="G13" s="11"/>
@@ -33110,9 +33119,9 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="vLKrgujUJur/R2VKGH5SPssphakl7sYVgML9xsXVSfEjOgKPyX8ZYl9Ms7FELh47m7qYAgVJY85AAI42aazRBQ==" saltValue="qNDLEUXOsR2BQODc3+z9OA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="td87MFi//N0oYbQW4FJqL8KHKjtLjyXOQv2Fnj8k3s/V3M5Tjmv2Lswe/OUvHQaRFO7OxnToTfhNe1utLJth+w==" saltValue="PLNJ2vzx4pBzTE1EXYs3lA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="69" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="69" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -33467,7 +33476,7 @@
       <c r="G17" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="+lLKajOHd3Z2ZZ4QE851L84jwillH2tSq3/zAnFPVNbBfSso0VAgQwcaOIy/wIeXO/NelJZRx+aBM4Tu+59QkQ==" saltValue="DO2rHMHMOrUIEU2uVqwSxw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="w6cq8WBQPG4V3O3oEQK8MovICXrKeuZiAJ5DbXmpf48olf+bDVv24KPVPAdLJnawceWP08xvLTNg4Y+pvQKJSw==" saltValue="CiQcIJtsPjF4LibalgYv9g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -33573,7 +33582,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="720xgxQSfpBerQafNBaDjw7vbS9v3fu1dnZwbPkCJz+SMguBYz3DdVCuei+bg9h+nMo7XfJQPi5DOfjLf9nYmA==" saltValue="y3z62Q4expJt8qRogSKqNg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="U/eS5v7EXSmAn00lfyjl9tBmHxRjgMnb8NecugK1krTq5/YkdxYj/DYAILZvXsoYcLRWrFQles/NKKedqqZ2PQ==" saltValue="XQM2gTttGm0dcEf0MOxgGg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -33632,7 +33641,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="102" t="s">
         <v>134</v>
       </c>
@@ -33649,10 +33658,10 @@
       <c r="J2" s="104"/>
       <c r="K2" s="104"/>
     </row>
-    <row r="3" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="103"/>
     </row>
-    <row r="4" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="102" t="s">
         <v>135</v>
       </c>
@@ -33669,10 +33678,10 @@
       <c r="J4" s="104"/>
       <c r="K4" s="104"/>
     </row>
-    <row r="5" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="103"/>
     </row>
-    <row r="6" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="102" t="s">
         <v>136</v>
       </c>
@@ -33689,7 +33698,7 @@
       <c r="J6" s="104"/>
       <c r="K6" s="104"/>
     </row>
-    <row r="7" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="103" t="s">
         <v>100</v>
       </c>
@@ -33703,7 +33712,7 @@
       <c r="J7" s="104"/>
       <c r="K7" s="104"/>
     </row>
-    <row r="8" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="103" t="s">
         <v>137</v>
       </c>
@@ -33717,7 +33726,7 @@
       <c r="J8" s="104"/>
       <c r="K8" s="104"/>
     </row>
-    <row r="10" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="102" t="s">
         <v>138</v>
       </c>
@@ -33734,7 +33743,7 @@
       <c r="J10" s="104"/>
       <c r="K10" s="104"/>
     </row>
-    <row r="11" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="103" t="s">
         <v>140</v>
       </c>
@@ -33748,7 +33757,7 @@
       <c r="J11" s="104"/>
       <c r="K11" s="104"/>
     </row>
-    <row r="13" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="102" t="s">
         <v>43</v>
       </c>
@@ -33765,7 +33774,7 @@
       <c r="J13" s="104"/>
       <c r="K13" s="104"/>
     </row>
-    <row r="14" spans="1:11" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="103" t="s">
         <v>142</v>
       </c>
@@ -33780,7 +33789,7 @@
       <c r="K14" s="104"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="F+fWtnmwpt3prV0dhm8TIIQA+YSiNzSiEbxgVS9S6M+EDq44tm3azdLd1wKx4apqMs7M/2AaQEntQNikEOg1bA==" saltValue="yOEjyPy5rRj26aeQ6ZCPuQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="eEaq4hwW/7e1l0vgbDNS3fajfYElkaGLTQrhaGPWzfbsDZQA6uUfkYbekVlUjlGgels2B0wd9wD+0wcAuUqrEw==" saltValue="tMrFjEneTaTJqXNQIQdQtg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="193" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -33812,7 +33821,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="102" t="s">
         <v>145</v>
       </c>
@@ -33820,7 +33829,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="102" t="s">
         <v>150</v>
       </c>
@@ -33828,7 +33837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="102" t="s">
         <v>146</v>
       </c>
@@ -33836,7 +33845,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="102" t="s">
         <v>147</v>
       </c>
@@ -33844,7 +33853,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="102" t="s">
         <v>148</v>
       </c>
@@ -33852,7 +33861,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="102" t="s">
         <v>149</v>
       </c>
@@ -33861,7 +33870,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Hr0Pb8xzXAhX3uYGJZ8B6aGPEkKtGpWoccBzgo6LElNN2hHzkPKiNyKKaGgI9em4r9kDJie+5KAt8ILvBG6aAQ==" saltValue="SeJ0mHJu9ka1+MLpx8D/Bg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2LOBj/YpdhPHKw+5sgkLSzz2VLKrC3x/aNw1L8Ryv1vsmfbhBw9S3GiII73SlR0WhBuo5PwFCWEkyaHS0i9FUA==" saltValue="nzThz533uEgQeDoJWgS2qA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -33917,7 +33926,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>109</v>
       </c>
@@ -33930,7 +33939,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="22" t="s">
         <v>96</v>
       </c>
@@ -33943,7 +33952,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="22" t="s">
         <v>97</v>
       </c>
@@ -33956,7 +33965,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="22" t="s">
         <v>98</v>
       </c>
@@ -33969,7 +33978,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="22" t="s">
         <v>156</v>
       </c>
@@ -33991,7 +34000,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="22" t="s">
         <v>109</v>
       </c>
@@ -34004,7 +34013,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="22" t="s">
         <v>96</v>
       </c>
@@ -34017,7 +34026,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="22" t="s">
         <v>97</v>
       </c>
@@ -34030,7 +34039,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="22" t="s">
         <v>98</v>
       </c>
@@ -34043,7 +34052,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="22" t="s">
         <v>156</v>
       </c>
@@ -34065,7 +34074,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="22" t="s">
         <v>109</v>
       </c>
@@ -34078,7 +34087,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="22" t="s">
         <v>96</v>
       </c>
@@ -34091,7 +34100,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="22" t="s">
         <v>97</v>
       </c>
@@ -34102,7 +34111,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="22" t="s">
         <v>98</v>
       </c>
@@ -34113,7 +34122,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="13.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="22" t="s">
         <v>156</v>
       </c>
@@ -34122,7 +34131,7 @@
       <c r="E21" s="42"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="NQe0nSRZugPt6MdzLHJs69wVXxfGxfeZxhNvDeuunYsK1Prk8tss4BV9cr1xi8tadtyxiOujUUjNrWbEuM/W6w==" saltValue="drzXdxAznpv9e/db28kLJg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="poui83KaCBAoKYyXFS/EBJrduA72lo3izQaITvLoutcBuutY6Xaf0EMEYDdZP5CtZYUtsOsa4m4nsQ56ifyN1A==" saltValue="RHpP1NO8c7Y3zlqmzK+AMw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -34186,7 +34195,7 @@
       <c r="D3" s="42"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="OFtXl5+1wt5cw+AqBUcD0lnUiQ93LvTw6V58CRnEeEsxcPRpSmlMyLcnqpXl/NYVrZx7dBQ46nDhe/wQKWj3Ng==" saltValue="mVY9/Vc9o55Ay6JRiLZTxw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="XHIUVwXG2IIwH1pYQNEOoouQVVv5UB2RghLIfz0GSfVSCAgUf0tXcaQIjxcFSK7CzBrJxKfLku1n2lMB2Itehg==" saltValue="VwWo/otmT96NRdsZ1OFKeQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix translation script capitalization
</commit_message>
<xml_diff>
--- a/inputs/fr/Optima_template.xlsx
+++ b/inputs/fr/Optima_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\romesh\projects\nutrition\inputs\fr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCFD3FC3-4421-45FD-93F2-6751DFCCED24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFDA34C0-CBCC-4760-B6B0-594646E7DAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="31920" windowHeight="14040" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2760" yWindow="6840" windowWidth="31920" windowHeight="14040" tabRatio="961" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Données pop de l'année de ref" sheetId="1" r:id="rId1"/>
@@ -410,7 +410,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2093" uniqueCount="337">
   <si>
     <t>Field</t>
   </si>
@@ -616,9 +616,6 @@
     <t>Insuffisance pondérale à la naissance</t>
   </si>
   <si>
-    <t>Année</t>
-  </si>
-  <si>
     <t>Nombre de naissances</t>
   </si>
   <si>
@@ -641,6 +638,9 @@
   </si>
   <si>
     <t>FAP non enceintes</t>
+  </si>
+  <si>
+    <t>année</t>
   </si>
   <si>
     <t>Néonatal</t>
@@ -1057,7 +1057,7 @@
     <t>En forme de S (coût marginal décroissant puis croissant)</t>
   </si>
   <si>
-    <t>efficacité</t>
+    <t>Efficacité</t>
   </si>
   <si>
     <t>Méthode</t>
@@ -1363,6 +1363,9 @@
     <t>Petite quantité de supplémentation en nutriments à base de lipids - supérieur</t>
   </si>
   <si>
+    <t>efficacité</t>
+  </si>
+  <si>
     <t>fraction touchée</t>
   </si>
   <si>
@@ -1411,6 +1414,9 @@
     <t>Condition ciblée</t>
   </si>
   <si>
+    <t>Fraction touchée</t>
+  </si>
+  <si>
     <t>Efficacité à prévenir une mort</t>
   </si>
   <si>
@@ -1428,7 +1434,7 @@
     <numFmt numFmtId="167" formatCode="0.0%"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1544,12 +1550,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1695,7 +1695,7 @@
     <xf numFmtId="9" fontId="18" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1941,9 +1941,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2710,7 +2707,7 @@
       <c r="A63" s="52"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Rvs3Xj7W5cSSMz673r+7+IsHFYyQ6gDcQAUEoCIrfzSkGBM93dwwaK+Sm0A3dDkHFxiE0DSQgRGKUst/R7DSMw==" saltValue="jolCXBSO+vLftebgowQBcw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+ZSqzfzK6B7JL74+aSKq0+ZbXN/xaSxvvLJCYtAl8hyeACEKg7Bz8v5s2eSirjfG/uuG/tVfSDAcFaST2YXJ/g==" saltValue="+ra48uFnx2CvcQ/LVCa0pQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -3488,7 +3485,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="HrJORgfSlocbXoJeRb/3i0QFDfDkZlHiCD04OBTg9ITDfiW/M2o+LaTsyRBKRbyuaOi+OB8bGN3w5wtDZgQVLQ==" saltValue="78ZobE1RRToFm5tlce0IzQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="vKUoypYNW8+9WUVb/3ngrS3IRBvIfr+mS0wfI+/pPmkjrt061HBmv4jtVRPqe94vr4YRHegYyGV6mEq5sDwTbg==" saltValue="oIlrHyfdK4Sud/zYRXNTVg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -3638,7 +3635,7 @@
       <c r="C20" s="45"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rvUB+mG7nanaP/8rlHcs5xa0xQVAtyi9PSccVqJoOhgX93IoBGcqgZ70LmnCiTLiBH1yA9m4cWD1R6ukrrxQSw==" saltValue="CYlw+Iv4mS7gkvHxChv5uQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="fRmIXhL1H1d87yhqaGVlLSUnfmFpC867WdErH/a82CEPfMIyK+xo7IUM+fwdueXbV9JP2esJnaudbh6Hcsd6cg==" saltValue="iSMdOEZf4nZolNHFGmTEvw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
@@ -3739,7 +3736,7 @@
       <c r="A19" s="23"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="i1HLlcAw6tpJjzUKrz1LCe0VaVwTV5Ej42TKb9UQBtUS3TXKQkfQL7Fi5Y7HL4LzGcz9sxSKMBHASpNq0shzgg==" saltValue="bqQ1Z31AL3DPd8nxry5nug==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="E7NNf6a6BPxU8FqLeguS9VRl+9vF4dox4j9d2DOLzXEA+8ymCyWHhbO0b+KoFn2PsI0s5YUiacspYTx7JP8Y3w==" saltValue="cRyE6sCq3pf5IejoskwBFA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -3854,7 +3851,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="P3ga6uGgyzWLSTAFFbesCjQU+UCZRsOnFV79iFkTcckRJNaHVK0ZRcki1bw4Mxb3dC0ry2Llh0Qm9jUf5SyNwg==" saltValue="lLt19OLzfh/TNEVW2We+SA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="mGfNm/YpzEaZKLE4bwrZRnffptUEkzpgHBXIR+I42mMdADJNepOAhUOXHFXXrN8NeMhLgzHCBas5a71O9CvBzQ==" saltValue="pKrmle6SHQ21tc00igc3Kw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -3918,16 +3915,16 @@
         <v>125</v>
       </c>
       <c r="L1" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="N1" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="O1" s="52" t="s">
         <v>72</v>
-      </c>
-      <c r="O1" s="52" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -4874,7 +4871,7 @@
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B24" s="65" t="s">
         <v>172</v>
@@ -5615,7 +5612,7 @@
       <c r="B40" s="17"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="e2WKKnloKyzCf162L1fZxncn0s5HuIC/eEx3/uHpR1seaDq++Y49WoLszkcozEPW2BFWG1IqkAgUIROvhYvHtg==" saltValue="yGbSqtn4zIp2gETZATVjGA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="qisl10VUBebpCiv8MkRpcrLtMwUa0kUtmp8Lineh3LjgrSqjAVrd88IWN//N2Bp+KPvJ37EptPB+lt9xy5dzIw==" saltValue="xZssUTCDmzzPa4mojNhsng==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -5650,7 +5647,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IuuaX4okD1Hq7Ixnq/lztwYllN4LRFGJJp+/5A9YGlKLXCmfS+RPkoOFFNHIAChKoPZahO51F7uGJUlUp6bpuA==" saltValue="QGDfkw4DayaGBucH+tgM3w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="nKmdsAXkRn0+Zhb4XjO9uKuA8R8AdsDgzG9nWUEMIC+Ryq9OLM2gvdJrHwwo0Kr6NnkFAjW76wOanfEfKehZxw==" saltValue="+B/4/YHS5QXVUcyybCeSKg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5856,7 +5853,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="uoQeN59GjYfO1dN7SsezqMm64eE5vbSKvlrpUGIpYYI5fz4B6gdJgF2iQepdF9M+DaA2fQMnmYlVeKFtLAPI+A==" saltValue="Zfyo0xtSsSWseR5AHJ847g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="q975wXiK+P2PbugbLUHyQfPAy2ySYPGvCL6d30PdlCTcz/K5oK4Qr17axaM7ZqEIO80q1PSilJ5nbLEJPirxPA==" saltValue="IZaNI5S6dlILcqSucmB6/Q==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -5923,16 +5920,16 @@
         <v>125</v>
       </c>
       <c r="L1" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="M1" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="52" t="s">
+      <c r="N1" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="52" t="s">
+      <c r="O1" s="52" t="s">
         <v>72</v>
-      </c>
-      <c r="O1" s="52" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6988,7 +6985,7 @@
     </row>
     <row r="27" spans="1:16" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="52" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B27" s="69" t="s">
         <v>172</v>
@@ -7671,7 +7668,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="CzDmDYmiNTFJGA6GQNEWPSlXqXjv3/UndViAC3THgMDtAYzjyAlHhLTHNJm+DTwNpVLkFKH5hyLXlOpTxaBNsg==" saltValue="mIwlXfIcFOn8UAoZaob9bA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="J3+2FSDz0+jixnuJGaV7kFSbLbWaEZ4p/T9eflU+unqhU5rNLXEjQpHzvBB+b4Qls1s6NuIIKXs0/xMnoExKlA==" saltValue="xJ1ykw1SWcXyE0HlBYhLbA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7735,7 +7732,7 @@
         <v>36</v>
       </c>
       <c r="K1" s="96" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -8439,7 +8436,7 @@
       <c r="K39" s="82"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="jaKHjV1cF7oXeLdAxDPLGUH9RGAzXGZdzfIrlq8Qb7aQ79yI1RWbwKe8QLJWQhDv/LOGCuxafG/+jukALMUHxQ==" saltValue="54qztp3Evrj2fkvBC2usCw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="DmQckkAQcyK/x+/kwWwogQBuzX3C1Kzbxk37KaG4kIaAfIY0sfH3S6luacDIO1HNlgfDPTQ29I6qknNjTKP7NA==" saltValue="4epw4C0N/hFs/CR6LgyccQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8503,7 +8500,7 @@
         <v>36</v>
       </c>
       <c r="K1" s="96" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -8737,7 +8734,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="96" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" s="82"/>
       <c r="C11" s="82" t="s">
@@ -8758,7 +8755,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="96" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="82"/>
       <c r="C12" s="82" t="s">
@@ -8777,7 +8774,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="96" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="82"/>
       <c r="C13" s="82" t="s">
@@ -8796,7 +8793,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="96" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B14" s="82"/>
       <c r="C14" s="82" t="s">
@@ -8814,7 +8811,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="opHwrTlJhtOuzZJI4IJIEdAfJhZhbIM3FYlFDYfbgRLG3Xq1Nxm8ohBoI6PUi6LV0yIs2mAVV1M1L833vesvTQ==" saltValue="fpkDjkxkpKhvImr3rpdJCQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="O1OUtw4sFp4H7RzG06vgam2NpBBLTMs5V1u0jP4fEqu6Ln/+fzn44QFvf60aXjp3F2ImFrQ8EMa0NT5POfMNWA==" saltValue="e2l+WZQ1EMHhsOcsIvEgMw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8840,31 +8837,31 @@
   <sheetData>
     <row r="1" spans="1:9" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="10" t="s">
         <v>75</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9804,7 +9801,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="rlB6WA8sAoJcyYXdsbcOv3EOhLaWIuwjP4+3kj+uVUBXWreKIoaGJh+h5OJvieJyDiBFzjrtLtY3efWXPF1fTQ==" saltValue="HhsqiIwCQm81V64GXff/XA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="KwQSo0K74u19xlQIvZ7zmTHcuZ6dAcyTLIk+O4sJsTZg8HUZqIKMS/4ZjPWJQ5SmMcnPVs9TMt+j7GvqWVOUJw==" saltValue="+CFHIAo3qor9qch3lwVkag==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="B2:I16 B18:I40 B17:C17 E17:I17">
     <cfRule type="expression" dxfId="0" priority="9">
       <formula>$A2=""</formula>
@@ -9865,7 +9862,7 @@
       <c r="A2" s="52" t="s">
         <v>232</v>
       </c>
-      <c r="B2" s="107" t="s">
+      <c r="B2" s="106" t="s">
         <v>100</v>
       </c>
       <c r="C2" s="96" t="s">
@@ -9888,7 +9885,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="108"/>
+      <c r="B3" s="107"/>
       <c r="C3" s="96" t="s">
         <v>154</v>
       </c>
@@ -9910,7 +9907,7 @@
       <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="108"/>
+      <c r="B4" s="107"/>
       <c r="C4" s="96" t="s">
         <v>155</v>
       </c>
@@ -9932,7 +9929,7 @@
       <c r="J4" s="53"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="106" t="s">
         <v>109</v>
       </c>
       <c r="C5" s="96" t="s">
@@ -9956,7 +9953,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="108"/>
+      <c r="B6" s="107"/>
       <c r="C6" s="96" t="s">
         <v>154</v>
       </c>
@@ -9977,7 +9974,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="108"/>
+      <c r="B7" s="107"/>
       <c r="C7" s="96" t="s">
         <v>155</v>
       </c>
@@ -9998,7 +9995,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="107" t="s">
+      <c r="B8" s="106" t="s">
         <v>96</v>
       </c>
       <c r="C8" s="96" t="s">
@@ -10021,7 +10018,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="108"/>
+      <c r="B9" s="107"/>
       <c r="C9" s="96" t="s">
         <v>154</v>
       </c>
@@ -10042,7 +10039,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B10" s="108"/>
+      <c r="B10" s="107"/>
       <c r="C10" s="96" t="s">
         <v>155</v>
       </c>
@@ -10063,7 +10060,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="107" t="s">
+      <c r="B11" s="106" t="s">
         <v>97</v>
       </c>
       <c r="C11" s="96" t="s">
@@ -10086,7 +10083,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="108"/>
+      <c r="B12" s="107"/>
       <c r="C12" s="96" t="s">
         <v>154</v>
       </c>
@@ -10107,7 +10104,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="108"/>
+      <c r="B13" s="107"/>
       <c r="C13" s="96" t="s">
         <v>155</v>
       </c>
@@ -10128,7 +10125,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="107" t="s">
+      <c r="B14" s="106" t="s">
         <v>98</v>
       </c>
       <c r="C14" s="96" t="s">
@@ -10151,7 +10148,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="108"/>
+      <c r="B15" s="107"/>
       <c r="C15" s="96" t="s">
         <v>154</v>
       </c>
@@ -10172,7 +10169,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="108"/>
+      <c r="B16" s="107"/>
       <c r="C16" s="96" t="s">
         <v>155</v>
       </c>
@@ -10226,7 +10223,7 @@
       <c r="A19" s="52" t="s">
         <v>233</v>
       </c>
-      <c r="B19" s="107" t="s">
+      <c r="B19" s="106" t="s">
         <v>100</v>
       </c>
       <c r="C19" s="96" t="s">
@@ -10249,7 +10246,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B20" s="108"/>
+      <c r="B20" s="107"/>
       <c r="C20" s="96" t="s">
         <v>154</v>
       </c>
@@ -10270,7 +10267,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B21" s="108"/>
+      <c r="B21" s="107"/>
       <c r="C21" s="96" t="s">
         <v>155</v>
       </c>
@@ -10291,7 +10288,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B22" s="107" t="s">
+      <c r="B22" s="106" t="s">
         <v>109</v>
       </c>
       <c r="C22" s="96" t="s">
@@ -10314,7 +10311,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B23" s="108"/>
+      <c r="B23" s="107"/>
       <c r="C23" s="96" t="s">
         <v>154</v>
       </c>
@@ -10335,7 +10332,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B24" s="108"/>
+      <c r="B24" s="107"/>
       <c r="C24" s="96" t="s">
         <v>155</v>
       </c>
@@ -10356,7 +10353,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B25" s="107" t="s">
+      <c r="B25" s="106" t="s">
         <v>96</v>
       </c>
       <c r="C25" s="96" t="s">
@@ -10379,7 +10376,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B26" s="108"/>
+      <c r="B26" s="107"/>
       <c r="C26" s="96" t="s">
         <v>154</v>
       </c>
@@ -10400,7 +10397,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B27" s="108"/>
+      <c r="B27" s="107"/>
       <c r="C27" s="96" t="s">
         <v>155</v>
       </c>
@@ -10421,7 +10418,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B28" s="107" t="s">
+      <c r="B28" s="106" t="s">
         <v>97</v>
       </c>
       <c r="C28" s="96" t="s">
@@ -10444,7 +10441,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B29" s="108"/>
+      <c r="B29" s="107"/>
       <c r="C29" s="96" t="s">
         <v>154</v>
       </c>
@@ -10465,7 +10462,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B30" s="108"/>
+      <c r="B30" s="107"/>
       <c r="C30" s="96" t="s">
         <v>155</v>
       </c>
@@ -10486,7 +10483,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B31" s="107" t="s">
+      <c r="B31" s="106" t="s">
         <v>98</v>
       </c>
       <c r="C31" s="96" t="s">
@@ -10509,7 +10506,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B32" s="108"/>
+      <c r="B32" s="107"/>
       <c r="C32" s="96" t="s">
         <v>154</v>
       </c>
@@ -10530,7 +10527,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B33" s="108"/>
+      <c r="B33" s="107"/>
       <c r="C33" s="96" t="s">
         <v>155</v>
       </c>
@@ -10584,7 +10581,7 @@
       <c r="A36" s="54" t="s">
         <v>234</v>
       </c>
-      <c r="B36" s="107" t="s">
+      <c r="B36" s="106" t="s">
         <v>100</v>
       </c>
       <c r="C36" s="96" t="s">
@@ -10607,7 +10604,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B37" s="108"/>
+      <c r="B37" s="107"/>
       <c r="C37" s="96" t="s">
         <v>154</v>
       </c>
@@ -10628,7 +10625,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B38" s="108"/>
+      <c r="B38" s="107"/>
       <c r="C38" s="96" t="s">
         <v>155</v>
       </c>
@@ -10649,7 +10646,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B39" s="107" t="s">
+      <c r="B39" s="106" t="s">
         <v>109</v>
       </c>
       <c r="C39" s="96" t="s">
@@ -10672,7 +10669,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B40" s="108"/>
+      <c r="B40" s="107"/>
       <c r="C40" s="96" t="s">
         <v>154</v>
       </c>
@@ -10693,7 +10690,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="108"/>
+      <c r="B41" s="107"/>
       <c r="C41" s="96" t="s">
         <v>155</v>
       </c>
@@ -10714,7 +10711,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="107" t="s">
+      <c r="B42" s="106" t="s">
         <v>96</v>
       </c>
       <c r="C42" s="96" t="s">
@@ -10737,7 +10734,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="108"/>
+      <c r="B43" s="107"/>
       <c r="C43" s="96" t="s">
         <v>154</v>
       </c>
@@ -10758,7 +10755,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="108"/>
+      <c r="B44" s="107"/>
       <c r="C44" s="96" t="s">
         <v>155</v>
       </c>
@@ -10779,7 +10776,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="107" t="s">
+      <c r="B45" s="106" t="s">
         <v>97</v>
       </c>
       <c r="C45" s="96" t="s">
@@ -10802,7 +10799,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B46" s="108"/>
+      <c r="B46" s="107"/>
       <c r="C46" s="96" t="s">
         <v>154</v>
       </c>
@@ -10823,7 +10820,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B47" s="108"/>
+      <c r="B47" s="107"/>
       <c r="C47" s="96" t="s">
         <v>155</v>
       </c>
@@ -10844,7 +10841,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B48" s="107" t="s">
+      <c r="B48" s="106" t="s">
         <v>98</v>
       </c>
       <c r="C48" s="96" t="s">
@@ -10867,7 +10864,7 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B49" s="108"/>
+      <c r="B49" s="107"/>
       <c r="C49" s="96" t="s">
         <v>154</v>
       </c>
@@ -10888,7 +10885,7 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B50" s="108"/>
+      <c r="B50" s="107"/>
       <c r="C50" s="96" t="s">
         <v>155</v>
       </c>
@@ -10973,7 +10970,7 @@
       <c r="A55" s="52" t="s">
         <v>236</v>
       </c>
-      <c r="B55" s="107" t="s">
+      <c r="B55" s="106" t="s">
         <v>100</v>
       </c>
       <c r="C55" s="96" t="s">
@@ -11001,7 +10998,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B56" s="108"/>
+      <c r="B56" s="107"/>
       <c r="C56" s="96" t="s">
         <v>154</v>
       </c>
@@ -11027,7 +11024,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B57" s="108"/>
+      <c r="B57" s="107"/>
       <c r="C57" s="96" t="s">
         <v>155</v>
       </c>
@@ -11053,7 +11050,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B58" s="107" t="s">
+      <c r="B58" s="106" t="s">
         <v>109</v>
       </c>
       <c r="C58" s="96" t="s">
@@ -11081,7 +11078,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B59" s="108"/>
+      <c r="B59" s="107"/>
       <c r="C59" s="96" t="s">
         <v>154</v>
       </c>
@@ -11107,7 +11104,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B60" s="108"/>
+      <c r="B60" s="107"/>
       <c r="C60" s="96" t="s">
         <v>155</v>
       </c>
@@ -11133,7 +11130,7 @@
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B61" s="107" t="s">
+      <c r="B61" s="106" t="s">
         <v>96</v>
       </c>
       <c r="C61" s="96" t="s">
@@ -11161,7 +11158,7 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B62" s="108"/>
+      <c r="B62" s="107"/>
       <c r="C62" s="96" t="s">
         <v>154</v>
       </c>
@@ -11187,7 +11184,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B63" s="108"/>
+      <c r="B63" s="107"/>
       <c r="C63" s="96" t="s">
         <v>155</v>
       </c>
@@ -11213,7 +11210,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B64" s="107" t="s">
+      <c r="B64" s="106" t="s">
         <v>97</v>
       </c>
       <c r="C64" s="96" t="s">
@@ -11241,7 +11238,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B65" s="108"/>
+      <c r="B65" s="107"/>
       <c r="C65" s="96" t="s">
         <v>154</v>
       </c>
@@ -11267,7 +11264,7 @@
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B66" s="108"/>
+      <c r="B66" s="107"/>
       <c r="C66" s="96" t="s">
         <v>155</v>
       </c>
@@ -11293,7 +11290,7 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B67" s="107" t="s">
+      <c r="B67" s="106" t="s">
         <v>98</v>
       </c>
       <c r="C67" s="96" t="s">
@@ -11321,7 +11318,7 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B68" s="108"/>
+      <c r="B68" s="107"/>
       <c r="C68" s="96" t="s">
         <v>154</v>
       </c>
@@ -11347,7 +11344,7 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B69" s="108"/>
+      <c r="B69" s="107"/>
       <c r="C69" s="96" t="s">
         <v>155</v>
       </c>
@@ -11411,7 +11408,7 @@
       <c r="A72" s="52" t="s">
         <v>237</v>
       </c>
-      <c r="B72" s="107" t="s">
+      <c r="B72" s="106" t="s">
         <v>100</v>
       </c>
       <c r="C72" s="96" t="s">
@@ -11439,7 +11436,7 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B73" s="108"/>
+      <c r="B73" s="107"/>
       <c r="C73" s="96" t="s">
         <v>154</v>
       </c>
@@ -11465,7 +11462,7 @@
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B74" s="108"/>
+      <c r="B74" s="107"/>
       <c r="C74" s="96" t="s">
         <v>155</v>
       </c>
@@ -11491,7 +11488,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B75" s="107" t="s">
+      <c r="B75" s="106" t="s">
         <v>109</v>
       </c>
       <c r="C75" s="96" t="s">
@@ -11519,7 +11516,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B76" s="108"/>
+      <c r="B76" s="107"/>
       <c r="C76" s="96" t="s">
         <v>154</v>
       </c>
@@ -11545,7 +11542,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B77" s="108"/>
+      <c r="B77" s="107"/>
       <c r="C77" s="96" t="s">
         <v>155</v>
       </c>
@@ -11571,7 +11568,7 @@
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B78" s="107" t="s">
+      <c r="B78" s="106" t="s">
         <v>96</v>
       </c>
       <c r="C78" s="96" t="s">
@@ -11599,7 +11596,7 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B79" s="108"/>
+      <c r="B79" s="107"/>
       <c r="C79" s="96" t="s">
         <v>154</v>
       </c>
@@ -11625,7 +11622,7 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B80" s="108"/>
+      <c r="B80" s="107"/>
       <c r="C80" s="96" t="s">
         <v>155</v>
       </c>
@@ -11651,7 +11648,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B81" s="107" t="s">
+      <c r="B81" s="106" t="s">
         <v>97</v>
       </c>
       <c r="C81" s="96" t="s">
@@ -11679,7 +11676,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B82" s="108"/>
+      <c r="B82" s="107"/>
       <c r="C82" s="96" t="s">
         <v>154</v>
       </c>
@@ -11705,7 +11702,7 @@
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B83" s="108"/>
+      <c r="B83" s="107"/>
       <c r="C83" s="96" t="s">
         <v>155</v>
       </c>
@@ -11731,7 +11728,7 @@
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B84" s="107" t="s">
+      <c r="B84" s="106" t="s">
         <v>98</v>
       </c>
       <c r="C84" s="96" t="s">
@@ -11759,7 +11756,7 @@
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B85" s="108"/>
+      <c r="B85" s="107"/>
       <c r="C85" s="96" t="s">
         <v>154</v>
       </c>
@@ -11785,7 +11782,7 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B86" s="108"/>
+      <c r="B86" s="107"/>
       <c r="C86" s="96" t="s">
         <v>155</v>
       </c>
@@ -11849,7 +11846,7 @@
       <c r="A89" s="54" t="s">
         <v>238</v>
       </c>
-      <c r="B89" s="107" t="s">
+      <c r="B89" s="106" t="s">
         <v>100</v>
       </c>
       <c r="C89" s="96" t="s">
@@ -11877,7 +11874,7 @@
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B90" s="108"/>
+      <c r="B90" s="107"/>
       <c r="C90" s="96" t="s">
         <v>154</v>
       </c>
@@ -11903,7 +11900,7 @@
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B91" s="108"/>
+      <c r="B91" s="107"/>
       <c r="C91" s="96" t="s">
         <v>155</v>
       </c>
@@ -11929,7 +11926,7 @@
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B92" s="107" t="s">
+      <c r="B92" s="106" t="s">
         <v>109</v>
       </c>
       <c r="C92" s="96" t="s">
@@ -11957,7 +11954,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B93" s="108"/>
+      <c r="B93" s="107"/>
       <c r="C93" s="96" t="s">
         <v>154</v>
       </c>
@@ -11983,7 +11980,7 @@
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B94" s="108"/>
+      <c r="B94" s="107"/>
       <c r="C94" s="96" t="s">
         <v>155</v>
       </c>
@@ -12009,7 +12006,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B95" s="107" t="s">
+      <c r="B95" s="106" t="s">
         <v>96</v>
       </c>
       <c r="C95" s="96" t="s">
@@ -12037,7 +12034,7 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B96" s="108"/>
+      <c r="B96" s="107"/>
       <c r="C96" s="96" t="s">
         <v>154</v>
       </c>
@@ -12063,7 +12060,7 @@
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B97" s="108"/>
+      <c r="B97" s="107"/>
       <c r="C97" s="96" t="s">
         <v>155</v>
       </c>
@@ -12089,7 +12086,7 @@
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B98" s="107" t="s">
+      <c r="B98" s="106" t="s">
         <v>97</v>
       </c>
       <c r="C98" s="96" t="s">
@@ -12117,7 +12114,7 @@
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B99" s="108"/>
+      <c r="B99" s="107"/>
       <c r="C99" s="96" t="s">
         <v>154</v>
       </c>
@@ -12143,7 +12140,7 @@
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B100" s="108"/>
+      <c r="B100" s="107"/>
       <c r="C100" s="96" t="s">
         <v>155</v>
       </c>
@@ -12169,7 +12166,7 @@
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B101" s="107" t="s">
+      <c r="B101" s="106" t="s">
         <v>98</v>
       </c>
       <c r="C101" s="96" t="s">
@@ -12197,7 +12194,7 @@
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B102" s="108"/>
+      <c r="B102" s="107"/>
       <c r="C102" s="96" t="s">
         <v>154</v>
       </c>
@@ -12223,7 +12220,7 @@
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B103" s="108"/>
+      <c r="B103" s="107"/>
       <c r="C103" s="96" t="s">
         <v>155</v>
       </c>
@@ -12318,7 +12315,7 @@
       <c r="A108" s="52" t="s">
         <v>240</v>
       </c>
-      <c r="B108" s="107" t="s">
+      <c r="B108" s="106" t="s">
         <v>100</v>
       </c>
       <c r="C108" s="96" t="s">
@@ -12346,7 +12343,7 @@
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B109" s="108"/>
+      <c r="B109" s="107"/>
       <c r="C109" s="96" t="s">
         <v>154</v>
       </c>
@@ -12372,7 +12369,7 @@
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B110" s="108"/>
+      <c r="B110" s="107"/>
       <c r="C110" s="96" t="s">
         <v>155</v>
       </c>
@@ -12398,7 +12395,7 @@
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B111" s="107" t="s">
+      <c r="B111" s="106" t="s">
         <v>109</v>
       </c>
       <c r="C111" s="96" t="s">
@@ -12426,7 +12423,7 @@
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B112" s="108"/>
+      <c r="B112" s="107"/>
       <c r="C112" s="96" t="s">
         <v>154</v>
       </c>
@@ -12452,7 +12449,7 @@
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B113" s="108"/>
+      <c r="B113" s="107"/>
       <c r="C113" s="96" t="s">
         <v>155</v>
       </c>
@@ -12478,7 +12475,7 @@
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B114" s="107" t="s">
+      <c r="B114" s="106" t="s">
         <v>96</v>
       </c>
       <c r="C114" s="96" t="s">
@@ -12506,7 +12503,7 @@
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B115" s="108"/>
+      <c r="B115" s="107"/>
       <c r="C115" s="96" t="s">
         <v>154</v>
       </c>
@@ -12532,7 +12529,7 @@
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B116" s="108"/>
+      <c r="B116" s="107"/>
       <c r="C116" s="96" t="s">
         <v>155</v>
       </c>
@@ -12558,7 +12555,7 @@
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B117" s="107" t="s">
+      <c r="B117" s="106" t="s">
         <v>97</v>
       </c>
       <c r="C117" s="96" t="s">
@@ -12586,7 +12583,7 @@
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B118" s="108"/>
+      <c r="B118" s="107"/>
       <c r="C118" s="96" t="s">
         <v>154</v>
       </c>
@@ -12612,7 +12609,7 @@
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B119" s="108"/>
+      <c r="B119" s="107"/>
       <c r="C119" s="96" t="s">
         <v>155</v>
       </c>
@@ -12638,7 +12635,7 @@
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B120" s="107" t="s">
+      <c r="B120" s="106" t="s">
         <v>98</v>
       </c>
       <c r="C120" s="96" t="s">
@@ -12666,7 +12663,7 @@
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B121" s="108"/>
+      <c r="B121" s="107"/>
       <c r="C121" s="96" t="s">
         <v>154</v>
       </c>
@@ -12692,7 +12689,7 @@
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B122" s="108"/>
+      <c r="B122" s="107"/>
       <c r="C122" s="96" t="s">
         <v>155</v>
       </c>
@@ -12756,7 +12753,7 @@
       <c r="A125" s="52" t="s">
         <v>241</v>
       </c>
-      <c r="B125" s="107" t="s">
+      <c r="B125" s="106" t="s">
         <v>100</v>
       </c>
       <c r="C125" s="96" t="s">
@@ -12784,7 +12781,7 @@
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B126" s="108"/>
+      <c r="B126" s="107"/>
       <c r="C126" s="96" t="s">
         <v>154</v>
       </c>
@@ -12810,7 +12807,7 @@
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B127" s="108"/>
+      <c r="B127" s="107"/>
       <c r="C127" s="96" t="s">
         <v>155</v>
       </c>
@@ -12836,7 +12833,7 @@
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B128" s="107" t="s">
+      <c r="B128" s="106" t="s">
         <v>109</v>
       </c>
       <c r="C128" s="96" t="s">
@@ -12864,7 +12861,7 @@
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B129" s="108"/>
+      <c r="B129" s="107"/>
       <c r="C129" s="96" t="s">
         <v>154</v>
       </c>
@@ -12890,7 +12887,7 @@
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B130" s="108"/>
+      <c r="B130" s="107"/>
       <c r="C130" s="96" t="s">
         <v>155</v>
       </c>
@@ -12916,7 +12913,7 @@
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B131" s="107" t="s">
+      <c r="B131" s="106" t="s">
         <v>96</v>
       </c>
       <c r="C131" s="96" t="s">
@@ -12944,7 +12941,7 @@
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B132" s="108"/>
+      <c r="B132" s="107"/>
       <c r="C132" s="96" t="s">
         <v>154</v>
       </c>
@@ -12970,7 +12967,7 @@
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B133" s="108"/>
+      <c r="B133" s="107"/>
       <c r="C133" s="96" t="s">
         <v>155</v>
       </c>
@@ -12996,7 +12993,7 @@
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B134" s="107" t="s">
+      <c r="B134" s="106" t="s">
         <v>97</v>
       </c>
       <c r="C134" s="96" t="s">
@@ -13024,7 +13021,7 @@
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B135" s="108"/>
+      <c r="B135" s="107"/>
       <c r="C135" s="96" t="s">
         <v>154</v>
       </c>
@@ -13050,7 +13047,7 @@
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B136" s="108"/>
+      <c r="B136" s="107"/>
       <c r="C136" s="96" t="s">
         <v>155</v>
       </c>
@@ -13076,7 +13073,7 @@
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B137" s="107" t="s">
+      <c r="B137" s="106" t="s">
         <v>98</v>
       </c>
       <c r="C137" s="96" t="s">
@@ -13104,7 +13101,7 @@
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B138" s="108"/>
+      <c r="B138" s="107"/>
       <c r="C138" s="96" t="s">
         <v>154</v>
       </c>
@@ -13130,7 +13127,7 @@
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B139" s="108"/>
+      <c r="B139" s="107"/>
       <c r="C139" s="96" t="s">
         <v>155</v>
       </c>
@@ -13194,7 +13191,7 @@
       <c r="A142" s="54" t="s">
         <v>242</v>
       </c>
-      <c r="B142" s="107" t="s">
+      <c r="B142" s="106" t="s">
         <v>100</v>
       </c>
       <c r="C142" s="96" t="s">
@@ -13222,7 +13219,7 @@
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B143" s="108"/>
+      <c r="B143" s="107"/>
       <c r="C143" s="96" t="s">
         <v>154</v>
       </c>
@@ -13248,7 +13245,7 @@
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B144" s="108"/>
+      <c r="B144" s="107"/>
       <c r="C144" s="96" t="s">
         <v>155</v>
       </c>
@@ -13274,7 +13271,7 @@
       </c>
     </row>
     <row r="145" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B145" s="107" t="s">
+      <c r="B145" s="106" t="s">
         <v>109</v>
       </c>
       <c r="C145" s="96" t="s">
@@ -13302,7 +13299,7 @@
       </c>
     </row>
     <row r="146" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B146" s="108"/>
+      <c r="B146" s="107"/>
       <c r="C146" s="96" t="s">
         <v>154</v>
       </c>
@@ -13328,7 +13325,7 @@
       </c>
     </row>
     <row r="147" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B147" s="108"/>
+      <c r="B147" s="107"/>
       <c r="C147" s="96" t="s">
         <v>155</v>
       </c>
@@ -13354,7 +13351,7 @@
       </c>
     </row>
     <row r="148" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B148" s="107" t="s">
+      <c r="B148" s="106" t="s">
         <v>96</v>
       </c>
       <c r="C148" s="96" t="s">
@@ -13382,7 +13379,7 @@
       </c>
     </row>
     <row r="149" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B149" s="108"/>
+      <c r="B149" s="107"/>
       <c r="C149" s="96" t="s">
         <v>154</v>
       </c>
@@ -13408,7 +13405,7 @@
       </c>
     </row>
     <row r="150" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B150" s="108"/>
+      <c r="B150" s="107"/>
       <c r="C150" s="96" t="s">
         <v>155</v>
       </c>
@@ -13434,7 +13431,7 @@
       </c>
     </row>
     <row r="151" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B151" s="107" t="s">
+      <c r="B151" s="106" t="s">
         <v>97</v>
       </c>
       <c r="C151" s="96" t="s">
@@ -13462,7 +13459,7 @@
       </c>
     </row>
     <row r="152" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B152" s="108"/>
+      <c r="B152" s="107"/>
       <c r="C152" s="96" t="s">
         <v>154</v>
       </c>
@@ -13488,7 +13485,7 @@
       </c>
     </row>
     <row r="153" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B153" s="108"/>
+      <c r="B153" s="107"/>
       <c r="C153" s="96" t="s">
         <v>155</v>
       </c>
@@ -13514,7 +13511,7 @@
       </c>
     </row>
     <row r="154" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B154" s="107" t="s">
+      <c r="B154" s="106" t="s">
         <v>98</v>
       </c>
       <c r="C154" s="96" t="s">
@@ -13542,7 +13539,7 @@
       </c>
     </row>
     <row r="155" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B155" s="108"/>
+      <c r="B155" s="107"/>
       <c r="C155" s="96" t="s">
         <v>154</v>
       </c>
@@ -13568,7 +13565,7 @@
       </c>
     </row>
     <row r="156" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B156" s="108"/>
+      <c r="B156" s="107"/>
       <c r="C156" s="96" t="s">
         <v>155</v>
       </c>
@@ -13622,7 +13619,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8jchdAvyuzn159j8B5b5T5QUey9z4yeO6E9UZ4Bp8JsPTI2B/cNCmZYofT+5ogrC4v1S2fAPLjQH/KyG/KL9QA==" saltValue="JAidFjqUb6afkQLyymkuQQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="kC95r2NgyRXlyNtmfQN34XLhTLoE/SbAIZq1DQOgUx1cEgqxDiikFnRzxOiukxUV/hudBzPTFGsC5X669yAA2Q==" saltValue="qnCmONwwYhnuiWbtxMpeMw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="45">
     <mergeCell ref="B145:B147"/>
     <mergeCell ref="B148:B150"/>
@@ -14889,7 +14886,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="bOFCuzacpc1Pt/Mrq5k3go1ocmZQbUwHNL0pj405sgM1CzxEMz2vxxwGEGxVOGXIieU+6COIY8c8bVhcFTqSzQ==" saltValue="PwQZT+Nuk4SavZt0hh7sUw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="E8QEdOYgCBmVxStgGck2GqDPdKehELmChGxDGgFABPuQO7lWVEBv15TGwqq93ZRboP69jwloUGoc/8Ixa4gX8w==" saltValue="+u7MNkp9xUrH9pVUM0RYtg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -23028,7 +23025,7 @@
       <c r="I328" s="72"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="XZ/3HSX+LWqHsyboHs7FkkOCb13gXmE9v27QYoQ+vAYUuwU+FWDTJnpjceBdxCc5KlpCmRBSz3SEzDAd938FcA==" saltValue="6slku/XA/1tpx5gLyks++w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="+Aqu8wzxUavNlaNOfZffv8/JyQuzj7yhtQu/6veclfBRz13HhCoW/uMcOar3m7d+ppH3hcx2i47gjY9KxEoy8A==" saltValue="dRzUhBNHY0CFThA0FPUWjQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -23328,16 +23325,16 @@
     </row>
     <row r="20" spans="1:7" s="58" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="52" t="s">
+      <c r="E20" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="52" t="s">
+      <c r="F20" s="52" t="s">
         <v>72</v>
-      </c>
-      <c r="F20" s="52" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -23703,16 +23700,16 @@
       <c r="A43" s="58"/>
       <c r="B43" s="58"/>
       <c r="C43" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="D43" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="D43" s="52" t="s">
+      <c r="E43" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="E43" s="52" t="s">
+      <c r="F43" s="52" t="s">
         <v>72</v>
-      </c>
-      <c r="F43" s="52" t="s">
-        <v>73</v>
       </c>
       <c r="G43" s="58"/>
     </row>
@@ -24083,16 +24080,16 @@
       <c r="A66" s="58"/>
       <c r="B66" s="58"/>
       <c r="C66" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="D66" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="D66" s="52" t="s">
+      <c r="E66" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="E66" s="52" t="s">
+      <c r="F66" s="52" t="s">
         <v>72</v>
-      </c>
-      <c r="F66" s="52" t="s">
-        <v>73</v>
       </c>
       <c r="G66" s="58"/>
     </row>
@@ -24118,7 +24115,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="tUywp4/6OprbGawFdc7y78d4uG/8rKvkn1oLwCBCjmnGqJPjAY18qSKDiAkOa+u/npyF1Dl4y1I8pdaU9mSTlA==" saltValue="jxeKgo3gO+Pxya7D6+RkTA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="8+SPd4X+t+On3Ctujg4qZRpkEbOfuKkQ2AaNTbW4512D6CRxsfhjstYKuL2wHrYwdaLJznB9FUNUL/jtdo4a3A==" saltValue="jMV7xvLVGE+pOy8pVW170A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -24168,7 +24165,7 @@
         <v>168</v>
       </c>
       <c r="B2" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C2" s="85">
         <v>0.21</v>
@@ -24186,7 +24183,7 @@
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="69"/>
       <c r="B3" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C3" s="85">
         <v>1</v>
@@ -24206,7 +24203,7 @@
         <v>180</v>
       </c>
       <c r="B4" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C4" s="85">
         <v>0.15</v>
@@ -24224,7 +24221,7 @@
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="69"/>
       <c r="B5" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C5" s="85">
         <v>1</v>
@@ -24244,7 +24241,7 @@
         <v>181</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C6" s="85">
         <v>0.15</v>
@@ -24262,7 +24259,7 @@
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="69"/>
       <c r="B7" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C7" s="85">
         <v>1</v>
@@ -24282,7 +24279,7 @@
         <v>182</v>
       </c>
       <c r="B8" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C8" s="85">
         <v>0.35</v>
@@ -24300,7 +24297,7 @@
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="69"/>
       <c r="B9" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C9" s="85">
         <v>1</v>
@@ -24320,7 +24317,7 @@
         <v>186</v>
       </c>
       <c r="B10" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C10" s="85">
         <v>0.35</v>
@@ -24338,7 +24335,7 @@
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="69"/>
       <c r="B11" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C11" s="85">
         <v>1</v>
@@ -24358,7 +24355,7 @@
         <v>190</v>
       </c>
       <c r="B12" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C12" s="85">
         <v>0.23</v>
@@ -24376,7 +24373,7 @@
     <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="69"/>
       <c r="B13" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C13" s="85">
         <v>1</v>
@@ -24419,7 +24416,7 @@
         <v>168</v>
       </c>
       <c r="B17" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C17" s="85">
         <f t="shared" ref="C17:F28" si="0">C2*0.9</f>
@@ -24441,7 +24438,7 @@
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="69"/>
       <c r="B18" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C18" s="85">
         <f t="shared" si="0"/>
@@ -24465,7 +24462,7 @@
         <v>180</v>
       </c>
       <c r="B19" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C19" s="85">
         <f t="shared" si="0"/>
@@ -24487,7 +24484,7 @@
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="69"/>
       <c r="B20" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C20" s="85">
         <f t="shared" si="0"/>
@@ -24511,7 +24508,7 @@
         <v>181</v>
       </c>
       <c r="B21" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C21" s="85">
         <f t="shared" si="0"/>
@@ -24533,7 +24530,7 @@
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="69"/>
       <c r="B22" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C22" s="85">
         <f t="shared" si="0"/>
@@ -24557,7 +24554,7 @@
         <v>182</v>
       </c>
       <c r="B23" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C23" s="85">
         <f t="shared" si="0"/>
@@ -24579,7 +24576,7 @@
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="69"/>
       <c r="B24" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C24" s="85">
         <f t="shared" si="0"/>
@@ -24603,7 +24600,7 @@
         <v>186</v>
       </c>
       <c r="B25" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C25" s="85">
         <f t="shared" si="0"/>
@@ -24625,7 +24622,7 @@
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="69"/>
       <c r="B26" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C26" s="85">
         <f t="shared" si="0"/>
@@ -24649,7 +24646,7 @@
         <v>190</v>
       </c>
       <c r="B27" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C27" s="85">
         <f t="shared" si="0"/>
@@ -24671,7 +24668,7 @@
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="69"/>
       <c r="B28" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C28" s="85">
         <f t="shared" si="0"/>
@@ -24718,7 +24715,7 @@
         <v>168</v>
       </c>
       <c r="B32" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C32" s="85">
         <f t="shared" ref="C32:F43" si="1">C2*1.05</f>
@@ -24740,7 +24737,7 @@
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="69"/>
       <c r="B33" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C33" s="85">
         <f t="shared" si="1"/>
@@ -24764,7 +24761,7 @@
         <v>180</v>
       </c>
       <c r="B34" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C34" s="85">
         <f t="shared" si="1"/>
@@ -24786,7 +24783,7 @@
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="69"/>
       <c r="B35" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C35" s="85">
         <f t="shared" si="1"/>
@@ -24810,7 +24807,7 @@
         <v>181</v>
       </c>
       <c r="B36" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C36" s="85">
         <f t="shared" si="1"/>
@@ -24832,7 +24829,7 @@
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="69"/>
       <c r="B37" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C37" s="85">
         <f t="shared" si="1"/>
@@ -24856,7 +24853,7 @@
         <v>182</v>
       </c>
       <c r="B38" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C38" s="85">
         <f t="shared" si="1"/>
@@ -24878,7 +24875,7 @@
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="69"/>
       <c r="B39" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C39" s="85">
         <f t="shared" si="1"/>
@@ -24902,7 +24899,7 @@
         <v>186</v>
       </c>
       <c r="B40" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C40" s="85">
         <f t="shared" si="1"/>
@@ -24924,7 +24921,7 @@
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="69"/>
       <c r="B41" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C41" s="85">
         <f t="shared" si="1"/>
@@ -24948,7 +24945,7 @@
         <v>190</v>
       </c>
       <c r="B42" s="69" t="s">
-        <v>215</v>
+        <v>317</v>
       </c>
       <c r="C42" s="85">
         <f t="shared" si="1"/>
@@ -24970,7 +24967,7 @@
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="69"/>
       <c r="B43" s="69" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="C43" s="85">
         <f t="shared" si="1"/>
@@ -24990,7 +24987,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Mlx5V54ZPfL+DVCPnxZpL3lujAbsWRRrIBO6YTvE5ERLKV+80Z7EUVvwMRratpgQiooYgwSGq70df99ZZsakxA==" saltValue="o2e4WKEZlot0d01mS01ekA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ZzQSHzv0oht3/BJqJLVEP+O6un99DwK5/Axc3wMzWJp5pM7dNqGa/Fgn0frWiZcAlzJAOrWOZgTFKbWv1Hkx9A==" saltValue="pxM/g8uIupg9wZcata+86A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -25035,16 +25032,16 @@
         <v>99</v>
       </c>
       <c r="H1" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="J1" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="K1" s="57" t="s">
         <v>72</v>
-      </c>
-      <c r="K1" s="57" t="s">
-        <v>73</v>
       </c>
       <c r="L1" s="57" t="s">
         <v>122</v>
@@ -25061,7 +25058,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -25638,7 +25635,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="52" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B17" s="65"/>
     </row>
@@ -25842,16 +25839,16 @@
         <v>99</v>
       </c>
       <c r="H24" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="I24" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="I24" s="57" t="s">
+      <c r="J24" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="J24" s="57" t="s">
+      <c r="K24" s="57" t="s">
         <v>72</v>
-      </c>
-      <c r="K24" s="57" t="s">
-        <v>73</v>
       </c>
       <c r="L24" s="57" t="s">
         <v>122</v>
@@ -25868,7 +25865,7 @@
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="52" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -26614,7 +26611,7 @@
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="52" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="B40" s="65"/>
     </row>
@@ -26870,16 +26867,16 @@
         <v>99</v>
       </c>
       <c r="H47" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="I47" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="I47" s="57" t="s">
+      <c r="J47" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="J47" s="57" t="s">
+      <c r="K47" s="57" t="s">
         <v>72</v>
-      </c>
-      <c r="K47" s="57" t="s">
-        <v>73</v>
       </c>
       <c r="L47" s="57" t="s">
         <v>122</v>
@@ -26896,7 +26893,7 @@
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="52" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.2">
@@ -27642,7 +27639,7 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="52" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="B63" s="65"/>
     </row>
@@ -27875,7 +27872,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="hPMwvJ3+d60YXLomjsJHjN8l/qdaXd/os4Ejte9XrQ56AMY5MxvNDptJjHUbflZEmBYxdpTKYHMTzH4O6fVp6Q==" saltValue="AGzu5fkA4JWi5Lzl/EZrKw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="crP6e0JBStybG3MF5I/u6dTHtpd3zZyb7YJQCmZVzD77n+qPis+hhcJyIgiTDFTaRLgbLuYEZbN3YYCy9a9WFw==" saltValue="p/3PG2KYgPZ0dwamjcc8MA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -27922,7 +27919,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="52" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -27947,7 +27944,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="52" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="B4" s="65"/>
       <c r="C4" s="77"/>
@@ -27978,7 +27975,7 @@
     </row>
     <row r="7" spans="1:7" s="88" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="88" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -28002,7 +27999,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="52" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -28032,7 +28029,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="52" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="B11" s="65"/>
       <c r="C11" s="77"/>
@@ -28068,7 +28065,7 @@
     </row>
     <row r="14" spans="1:7" s="88" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="88" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -28092,7 +28089,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="52" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -28122,7 +28119,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="52" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B18" s="65"/>
       <c r="C18" s="77"/>
@@ -28157,7 +28154,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="J+vI+r+YzShTlBS6C9XfQQXNIJsXwjS4Kog7Au9WDfiXZljyR7MRofE0oFDb2JJRbHMKYt6rz4a4Oiun6HyUZQ==" saltValue="Jp3f4cwAN4uNFV/t6wUz+A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="tb0UfxW32mEr7nZHh+6Bur7q/AiLVfB5RxPQvU6dngRQUj6p+eNe3q+eR6j2DpZKtoJEvLA3y1/Kd8iFn81Xkg==" saltValue="dRIry6BHkcg36vvn7y8ICw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -28193,7 +28190,7 @@
         <v>160</v>
       </c>
       <c r="B1" s="52" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C1" s="76" t="s">
         <v>12</v>
@@ -28222,7 +28219,7 @@
         <v>87</v>
       </c>
       <c r="C2" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D2" s="85">
         <v>0</v>
@@ -28242,7 +28239,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C3" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D3" s="85">
         <v>0</v>
@@ -28262,7 +28259,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C4" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D4" s="85">
         <v>0</v>
@@ -28288,7 +28285,7 @@
         <v>208</v>
       </c>
       <c r="C5" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D5" s="85">
         <v>0</v>
@@ -28308,7 +28305,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C6" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D6" s="85">
         <v>0</v>
@@ -28331,7 +28328,7 @@
         <v>209</v>
       </c>
       <c r="C7" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D7" s="85">
         <v>0</v>
@@ -28351,7 +28348,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C8" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D8" s="85">
         <v>0</v>
@@ -28377,7 +28374,7 @@
         <v>208</v>
       </c>
       <c r="C9" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D9" s="85">
         <v>0</v>
@@ -28397,7 +28394,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D10" s="85">
         <v>0</v>
@@ -28420,7 +28417,7 @@
         <v>209</v>
       </c>
       <c r="C11" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D11" s="85">
         <v>0</v>
@@ -28440,7 +28437,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D12" s="85">
         <v>0</v>
@@ -28466,7 +28463,7 @@
         <v>208</v>
       </c>
       <c r="C13" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D13" s="85">
         <v>0</v>
@@ -28486,7 +28483,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C14" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D14" s="85">
         <v>0</v>
@@ -28509,7 +28506,7 @@
         <v>209</v>
       </c>
       <c r="C15" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D15" s="85">
         <v>0</v>
@@ -28529,7 +28526,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C16" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D16" s="85">
         <v>0</v>
@@ -28555,7 +28552,7 @@
         <v>208</v>
       </c>
       <c r="C17" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D17" s="85">
         <v>0</v>
@@ -28575,7 +28572,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C18" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D18" s="85">
         <v>0</v>
@@ -28598,7 +28595,7 @@
         <v>209</v>
       </c>
       <c r="C19" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D19" s="85">
         <v>0</v>
@@ -28618,7 +28615,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C20" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D20" s="85">
         <v>0</v>
@@ -28644,7 +28641,7 @@
         <v>84</v>
       </c>
       <c r="C21" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D21" s="85">
         <v>0.28260869565217389</v>
@@ -28664,7 +28661,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C22" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D22" s="85">
         <v>0.46</v>
@@ -28690,7 +28687,7 @@
         <v>84</v>
       </c>
       <c r="C23" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D23" s="85">
         <v>0.28260869565217389</v>
@@ -28710,7 +28707,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C24" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D24" s="85">
         <v>0.46</v>
@@ -28736,7 +28733,7 @@
         <v>84</v>
       </c>
       <c r="C25" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D25" s="85">
         <v>0.28260869565217389</v>
@@ -28756,7 +28753,7 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C26" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D26" s="85">
         <v>0.46</v>
@@ -28782,7 +28779,7 @@
         <v>87</v>
       </c>
       <c r="C27" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D27" s="85">
         <v>1</v>
@@ -28802,7 +28799,7 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C28" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D28" s="85">
         <v>0</v>
@@ -28822,7 +28819,7 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C29" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D29" s="85">
         <v>0</v>
@@ -28848,7 +28845,7 @@
         <v>87</v>
       </c>
       <c r="C30" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D30" s="85">
         <v>1</v>
@@ -28868,7 +28865,7 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C31" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D31" s="85">
         <v>0</v>
@@ -28888,7 +28885,7 @@
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C32" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D32" s="85">
         <v>0</v>
@@ -28914,7 +28911,7 @@
         <v>87</v>
       </c>
       <c r="C33" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D33" s="85">
         <v>1</v>
@@ -28934,7 +28931,7 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C34" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D34" s="85">
         <v>0</v>
@@ -28954,7 +28951,7 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C35" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D35" s="85">
         <v>0</v>
@@ -28980,7 +28977,7 @@
         <v>87</v>
       </c>
       <c r="C36" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D36" s="85">
         <v>1</v>
@@ -29000,7 +28997,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C37" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D37" s="85">
         <v>0</v>
@@ -29020,7 +29017,7 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C38" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D38" s="85">
         <v>0</v>
@@ -29046,7 +29043,7 @@
         <v>87</v>
       </c>
       <c r="C39" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D39" s="85">
         <v>1</v>
@@ -29066,7 +29063,7 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C40" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D40" s="85">
         <v>0</v>
@@ -29086,7 +29083,7 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C41" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D41" s="85">
         <v>0</v>
@@ -29112,7 +29109,7 @@
         <v>87</v>
       </c>
       <c r="C42" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D42" s="85">
         <v>0.3</v>
@@ -29132,7 +29129,7 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C43" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D43" s="85">
         <v>0.5</v>
@@ -29152,7 +29149,7 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C44" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D44" s="85">
         <v>0.65</v>
@@ -29175,7 +29172,7 @@
         <v>88</v>
       </c>
       <c r="C45" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D45" s="85">
         <v>0.3</v>
@@ -29195,7 +29192,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C46" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D46" s="85">
         <v>0.49</v>
@@ -29215,7 +29212,7 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C47" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D47" s="85">
         <v>0.52</v>
@@ -29241,7 +29238,7 @@
         <v>87</v>
       </c>
       <c r="C48" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D48" s="85">
         <v>0.88</v>
@@ -29261,7 +29258,7 @@
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C49" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D49" s="85">
         <v>0.78409090909090906</v>
@@ -29287,7 +29284,7 @@
         <v>87</v>
       </c>
       <c r="C50" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D50" s="85">
         <v>0.88372093023255816</v>
@@ -29307,7 +29304,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C51" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D51" s="85">
         <v>0.86</v>
@@ -29333,7 +29330,7 @@
         <v>82</v>
       </c>
       <c r="C52" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D52" s="85">
         <v>0.57999999999999996</v>
@@ -29353,7 +29350,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C53" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D53" s="85">
         <v>0.51</v>
@@ -29373,7 +29370,7 @@
     </row>
     <row r="55" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="92" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="B55" s="93"/>
       <c r="C55" s="93"/>
@@ -29383,7 +29380,7 @@
         <v>160</v>
       </c>
       <c r="B56" s="52" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C56" s="76" t="s">
         <v>12</v>
@@ -29412,7 +29409,7 @@
         <v>87</v>
       </c>
       <c r="C57" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D57" s="85">
         <f t="shared" ref="D57:H66" si="0">D2*0.9</f>
@@ -29437,7 +29434,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C58" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D58" s="85">
         <f t="shared" si="0"/>
@@ -29462,7 +29459,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C59" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D59" s="85">
         <f t="shared" si="0"/>
@@ -29493,7 +29490,7 @@
         <v>208</v>
       </c>
       <c r="C60" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D60" s="85">
         <f t="shared" si="0"/>
@@ -29518,7 +29515,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C61" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D61" s="85">
         <f t="shared" si="0"/>
@@ -29546,7 +29543,7 @@
         <v>209</v>
       </c>
       <c r="C62" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D62" s="85">
         <f t="shared" si="0"/>
@@ -29571,7 +29568,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C63" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D63" s="85">
         <f t="shared" si="0"/>
@@ -29602,7 +29599,7 @@
         <v>208</v>
       </c>
       <c r="C64" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D64" s="85">
         <f t="shared" si="0"/>
@@ -29627,7 +29624,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C65" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D65" s="85">
         <f t="shared" si="0"/>
@@ -29655,7 +29652,7 @@
         <v>209</v>
       </c>
       <c r="C66" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D66" s="85">
         <f t="shared" si="0"/>
@@ -29680,7 +29677,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C67" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D67" s="85">
         <f t="shared" ref="D67:H76" si="1">D12*0.9</f>
@@ -29711,7 +29708,7 @@
         <v>208</v>
       </c>
       <c r="C68" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D68" s="85">
         <f t="shared" si="1"/>
@@ -29736,7 +29733,7 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C69" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D69" s="85">
         <f t="shared" si="1"/>
@@ -29764,7 +29761,7 @@
         <v>209</v>
       </c>
       <c r="C70" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D70" s="85">
         <f t="shared" si="1"/>
@@ -29789,7 +29786,7 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C71" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D71" s="85">
         <f t="shared" si="1"/>
@@ -29820,7 +29817,7 @@
         <v>208</v>
       </c>
       <c r="C72" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D72" s="85">
         <f t="shared" si="1"/>
@@ -29845,7 +29842,7 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C73" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D73" s="85">
         <f t="shared" si="1"/>
@@ -29873,7 +29870,7 @@
         <v>209</v>
       </c>
       <c r="C74" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D74" s="85">
         <f t="shared" si="1"/>
@@ -29898,7 +29895,7 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C75" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D75" s="85">
         <f t="shared" si="1"/>
@@ -29929,7 +29926,7 @@
         <v>84</v>
       </c>
       <c r="C76" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D76" s="85">
         <f t="shared" si="1"/>
@@ -29954,7 +29951,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C77" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D77" s="85">
         <f t="shared" ref="D77:H86" si="2">D22*0.9</f>
@@ -29985,7 +29982,7 @@
         <v>84</v>
       </c>
       <c r="C78" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D78" s="85">
         <f t="shared" si="2"/>
@@ -30010,7 +30007,7 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C79" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D79" s="85">
         <f t="shared" si="2"/>
@@ -30041,7 +30038,7 @@
         <v>84</v>
       </c>
       <c r="C80" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D80" s="85">
         <f t="shared" si="2"/>
@@ -30066,7 +30063,7 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C81" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D81" s="85">
         <f t="shared" si="2"/>
@@ -30097,7 +30094,7 @@
         <v>87</v>
       </c>
       <c r="C82" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D82" s="85">
         <f t="shared" si="2"/>
@@ -30122,7 +30119,7 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C83" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D83" s="85">
         <f t="shared" si="2"/>
@@ -30147,7 +30144,7 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C84" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D84" s="85">
         <f t="shared" si="2"/>
@@ -30178,7 +30175,7 @@
         <v>87</v>
       </c>
       <c r="C85" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D85" s="85">
         <f t="shared" si="2"/>
@@ -30203,7 +30200,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C86" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D86" s="85">
         <f t="shared" si="2"/>
@@ -30228,7 +30225,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C87" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D87" s="85">
         <f t="shared" ref="D87:H96" si="3">D32*0.9</f>
@@ -30259,7 +30256,7 @@
         <v>87</v>
       </c>
       <c r="C88" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D88" s="85">
         <f t="shared" si="3"/>
@@ -30284,7 +30281,7 @@
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C89" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D89" s="85">
         <f t="shared" si="3"/>
@@ -30309,7 +30306,7 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C90" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D90" s="85">
         <f t="shared" si="3"/>
@@ -30340,7 +30337,7 @@
         <v>87</v>
       </c>
       <c r="C91" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D91" s="85">
         <f t="shared" si="3"/>
@@ -30365,7 +30362,7 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C92" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D92" s="85">
         <f t="shared" si="3"/>
@@ -30390,7 +30387,7 @@
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C93" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D93" s="85">
         <f t="shared" si="3"/>
@@ -30421,7 +30418,7 @@
         <v>87</v>
       </c>
       <c r="C94" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D94" s="85">
         <f t="shared" si="3"/>
@@ -30446,7 +30443,7 @@
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C95" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D95" s="85">
         <f t="shared" si="3"/>
@@ -30471,7 +30468,7 @@
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C96" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D96" s="85">
         <f t="shared" si="3"/>
@@ -30502,7 +30499,7 @@
         <v>87</v>
       </c>
       <c r="C97" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D97" s="85">
         <f t="shared" ref="D97:H106" si="4">D42*0.9</f>
@@ -30527,7 +30524,7 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C98" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D98" s="85">
         <f t="shared" si="4"/>
@@ -30552,7 +30549,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C99" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D99" s="85">
         <f t="shared" si="4"/>
@@ -30580,7 +30577,7 @@
         <v>88</v>
       </c>
       <c r="C100" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D100" s="85">
         <f t="shared" si="4"/>
@@ -30605,7 +30602,7 @@
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C101" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D101" s="85">
         <f t="shared" si="4"/>
@@ -30630,7 +30627,7 @@
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C102" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D102" s="85">
         <f t="shared" si="4"/>
@@ -30661,7 +30658,7 @@
         <v>87</v>
       </c>
       <c r="C103" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D103" s="85">
         <f t="shared" si="4"/>
@@ -30686,7 +30683,7 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C104" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D104" s="85">
         <f t="shared" si="4"/>
@@ -30717,7 +30714,7 @@
         <v>87</v>
       </c>
       <c r="C105" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D105" s="85">
         <f t="shared" si="4"/>
@@ -30742,7 +30739,7 @@
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C106" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D106" s="85">
         <f t="shared" si="4"/>
@@ -30773,7 +30770,7 @@
         <v>82</v>
       </c>
       <c r="C107" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D107" s="85">
         <f t="shared" ref="D107:H108" si="5">D52*0.9</f>
@@ -30798,7 +30795,7 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C108" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D108" s="85">
         <f t="shared" si="5"/>
@@ -30823,7 +30820,7 @@
     </row>
     <row r="110" spans="1:8" s="89" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A110" s="92" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="B110" s="93"/>
       <c r="C110" s="93"/>
@@ -30833,7 +30830,7 @@
         <v>160</v>
       </c>
       <c r="B111" s="52" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C111" s="76" t="s">
         <v>12</v>
@@ -30862,7 +30859,7 @@
         <v>87</v>
       </c>
       <c r="C112" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D112" s="85">
         <f t="shared" ref="D112:H121" si="6">D2*1.05</f>
@@ -30887,7 +30884,7 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C113" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D113" s="85">
         <f t="shared" si="6"/>
@@ -30912,7 +30909,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C114" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D114" s="85">
         <f t="shared" si="6"/>
@@ -30943,7 +30940,7 @@
         <v>208</v>
       </c>
       <c r="C115" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D115" s="85">
         <f t="shared" si="6"/>
@@ -30968,7 +30965,7 @@
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C116" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D116" s="85">
         <f t="shared" si="6"/>
@@ -30996,7 +30993,7 @@
         <v>209</v>
       </c>
       <c r="C117" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D117" s="85">
         <f t="shared" si="6"/>
@@ -31021,7 +31018,7 @@
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C118" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D118" s="85">
         <f t="shared" si="6"/>
@@ -31052,7 +31049,7 @@
         <v>208</v>
       </c>
       <c r="C119" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D119" s="85">
         <f t="shared" si="6"/>
@@ -31077,7 +31074,7 @@
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C120" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D120" s="85">
         <f t="shared" si="6"/>
@@ -31105,7 +31102,7 @@
         <v>209</v>
       </c>
       <c r="C121" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D121" s="85">
         <f t="shared" si="6"/>
@@ -31130,7 +31127,7 @@
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C122" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D122" s="85">
         <f t="shared" ref="D122:H131" si="7">D12*1.05</f>
@@ -31161,7 +31158,7 @@
         <v>208</v>
       </c>
       <c r="C123" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D123" s="85">
         <f t="shared" si="7"/>
@@ -31186,7 +31183,7 @@
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C124" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D124" s="85">
         <f t="shared" si="7"/>
@@ -31214,7 +31211,7 @@
         <v>209</v>
       </c>
       <c r="C125" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D125" s="85">
         <f t="shared" si="7"/>
@@ -31239,7 +31236,7 @@
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C126" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D126" s="85">
         <f t="shared" si="7"/>
@@ -31270,7 +31267,7 @@
         <v>208</v>
       </c>
       <c r="C127" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D127" s="85">
         <f t="shared" si="7"/>
@@ -31295,7 +31292,7 @@
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C128" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D128" s="85">
         <f t="shared" si="7"/>
@@ -31323,7 +31320,7 @@
         <v>209</v>
       </c>
       <c r="C129" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D129" s="85">
         <f t="shared" si="7"/>
@@ -31348,7 +31345,7 @@
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C130" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D130" s="85">
         <f t="shared" si="7"/>
@@ -31379,7 +31376,7 @@
         <v>84</v>
       </c>
       <c r="C131" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D131" s="85">
         <f t="shared" si="7"/>
@@ -31404,7 +31401,7 @@
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C132" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D132" s="85">
         <f t="shared" ref="D132:H141" si="8">D22*1.05</f>
@@ -31435,7 +31432,7 @@
         <v>84</v>
       </c>
       <c r="C133" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D133" s="85">
         <f t="shared" si="8"/>
@@ -31460,7 +31457,7 @@
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C134" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D134" s="85">
         <f t="shared" si="8"/>
@@ -31491,7 +31488,7 @@
         <v>84</v>
       </c>
       <c r="C135" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D135" s="85">
         <f t="shared" si="8"/>
@@ -31516,7 +31513,7 @@
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C136" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D136" s="85">
         <f t="shared" si="8"/>
@@ -31547,7 +31544,7 @@
         <v>87</v>
       </c>
       <c r="C137" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D137" s="85">
         <f t="shared" si="8"/>
@@ -31572,7 +31569,7 @@
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C138" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D138" s="85">
         <f t="shared" si="8"/>
@@ -31597,7 +31594,7 @@
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C139" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D139" s="85">
         <f t="shared" si="8"/>
@@ -31628,7 +31625,7 @@
         <v>87</v>
       </c>
       <c r="C140" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D140" s="85">
         <f t="shared" si="8"/>
@@ -31653,7 +31650,7 @@
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C141" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D141" s="85">
         <f t="shared" si="8"/>
@@ -31678,7 +31675,7 @@
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C142" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D142" s="85">
         <f t="shared" ref="D142:H151" si="9">D32*1.05</f>
@@ -31709,7 +31706,7 @@
         <v>87</v>
       </c>
       <c r="C143" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D143" s="85">
         <f t="shared" si="9"/>
@@ -31734,7 +31731,7 @@
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C144" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D144" s="85">
         <f t="shared" si="9"/>
@@ -31759,7 +31756,7 @@
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C145" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D145" s="85">
         <f t="shared" si="9"/>
@@ -31790,7 +31787,7 @@
         <v>87</v>
       </c>
       <c r="C146" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D146" s="85">
         <f t="shared" si="9"/>
@@ -31815,7 +31812,7 @@
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C147" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D147" s="85">
         <f t="shared" si="9"/>
@@ -31840,7 +31837,7 @@
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C148" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D148" s="85">
         <f t="shared" si="9"/>
@@ -31871,7 +31868,7 @@
         <v>87</v>
       </c>
       <c r="C149" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D149" s="85">
         <f t="shared" si="9"/>
@@ -31896,7 +31893,7 @@
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C150" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D150" s="85">
         <f t="shared" si="9"/>
@@ -31921,7 +31918,7 @@
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C151" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D151" s="85">
         <f t="shared" si="9"/>
@@ -31952,7 +31949,7 @@
         <v>87</v>
       </c>
       <c r="C152" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D152" s="85">
         <f t="shared" ref="D152:H161" si="10">D42*1.05</f>
@@ -31977,7 +31974,7 @@
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C153" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D153" s="85">
         <f t="shared" si="10"/>
@@ -32002,7 +31999,7 @@
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C154" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D154" s="85">
         <f t="shared" si="10"/>
@@ -32030,7 +32027,7 @@
         <v>88</v>
       </c>
       <c r="C155" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D155" s="85">
         <f t="shared" si="10"/>
@@ -32055,7 +32052,7 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C156" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D156" s="85">
         <f t="shared" si="10"/>
@@ -32080,7 +32077,7 @@
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C157" s="69" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D157" s="85">
         <f t="shared" si="10"/>
@@ -32111,7 +32108,7 @@
         <v>87</v>
       </c>
       <c r="C158" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D158" s="85">
         <f t="shared" si="10"/>
@@ -32136,7 +32133,7 @@
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C159" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D159" s="85">
         <f t="shared" si="10"/>
@@ -32167,7 +32164,7 @@
         <v>87</v>
       </c>
       <c r="C160" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D160" s="85">
         <f t="shared" si="10"/>
@@ -32192,7 +32189,7 @@
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C161" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D161" s="85">
         <f t="shared" si="10"/>
@@ -32223,7 +32220,7 @@
         <v>82</v>
       </c>
       <c r="C162" s="69" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D162" s="85">
         <f t="shared" ref="D162:H163" si="11">D52*1.05</f>
@@ -32248,7 +32245,7 @@
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C163" s="69" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D163" s="85">
         <f t="shared" si="11"/>
@@ -32272,7 +32269,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="lOinZ9WBtxvlmLsihEzxEIU5d+DHGJzI8KefS8dub44efJYhfBi7wNeWAGn4exxilOKuQ0dlz0LO6hftmolFmw==" saltValue="rbouoBWGwTxAgNQatjmjCg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="hCJB0TA1Wx1rco/NGCDm4kv0G4YYZxgnNvTJZYzid3cikpLsCs7UDhU2O7Mgs1npSx5wrP3GdD+kuqZUnn2yqA==" saltValue="010Z5WhAOC1F9wREhspcXA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -32304,7 +32301,7 @@
         <v>160</v>
       </c>
       <c r="B1" s="70" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C1" s="70"/>
       <c r="D1" s="52" t="s">
@@ -32329,7 +32326,7 @@
         <v>104</v>
       </c>
       <c r="C2" s="78" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D2" s="85">
         <v>1</v>
@@ -32347,7 +32344,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C3" s="96" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D3" s="85">
         <v>0.2</v>
@@ -32371,7 +32368,7 @@
         <v>104</v>
       </c>
       <c r="C4" s="78" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D4" s="85">
         <v>1</v>
@@ -32389,7 +32386,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C5" s="96" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D5" s="85">
         <v>0.59</v>
@@ -32413,7 +32410,7 @@
         <v>104</v>
       </c>
       <c r="C6" s="78" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D6" s="85">
         <v>1</v>
@@ -32431,7 +32428,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C7" s="96" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D7" s="85">
         <v>0.6</v>
@@ -32449,7 +32446,7 @@
     </row>
     <row r="9" spans="1:8" s="88" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="88" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
@@ -32457,7 +32454,7 @@
         <v>160</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C10" s="70"/>
       <c r="D10" s="52" t="s">
@@ -32481,7 +32478,7 @@
         <v>104</v>
       </c>
       <c r="C11" s="78" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D11" s="85">
         <f t="shared" ref="D11:G16" si="0">D2*0.9</f>
@@ -32502,7 +32499,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12" s="96" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D12" s="85">
         <f t="shared" si="0"/>
@@ -32529,7 +32526,7 @@
         <v>104</v>
       </c>
       <c r="C13" s="78" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D13" s="85">
         <f t="shared" si="0"/>
@@ -32550,7 +32547,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C14" s="96" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D14" s="85">
         <f t="shared" si="0"/>
@@ -32577,7 +32574,7 @@
         <v>104</v>
       </c>
       <c r="C15" s="78" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D15" s="85">
         <f t="shared" si="0"/>
@@ -32598,7 +32595,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C16" s="96" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D16" s="85">
         <f t="shared" si="0"/>
@@ -32619,7 +32616,7 @@
     </row>
     <row r="18" spans="1:7" s="88" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="88" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -32627,7 +32624,7 @@
         <v>160</v>
       </c>
       <c r="B19" s="70" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="C19" s="70"/>
       <c r="D19" s="52" t="s">
@@ -32651,7 +32648,7 @@
         <v>104</v>
       </c>
       <c r="C20" s="78" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D20" s="85">
         <f t="shared" ref="D20:G25" si="1">D2*1.05</f>
@@ -32672,7 +32669,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C21" s="96" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D21" s="85">
         <f t="shared" si="1"/>
@@ -32699,7 +32696,7 @@
         <v>104</v>
       </c>
       <c r="C22" s="78" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D22" s="85">
         <f t="shared" si="1"/>
@@ -32720,7 +32717,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C23" s="96" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D23" s="85">
         <f t="shared" si="1"/>
@@ -32747,7 +32744,7 @@
         <v>104</v>
       </c>
       <c r="C24" s="78" t="s">
-        <v>317</v>
+        <v>334</v>
       </c>
       <c r="D24" s="85">
         <f t="shared" si="1"/>
@@ -32768,7 +32765,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C25" s="96" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D25" s="85">
         <f t="shared" si="1"/>
@@ -32788,7 +32785,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Viu2TMxvPQIu38K1spqkyKyiRS85Gp3pyRsHsIb8yKqDoPGODNl1xxBk8+cCqYFNPc6Kg8ZYPXOLz7u8lnt2hA==" saltValue="aFHlcxl+SrVKrvwucWAL7A==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="AB7WiWQ07Mn3vzVQvtLAGHLW5n49MuWSs2dU7pRaiBbzmlBqGRQxNZ2qhb9keExW6c2ZWEq7B72yalqoolI65A==" saltValue="JaccJxbrWhkgAzWMySduoA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -32800,8 +32797,8 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:F13"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C11" activeCellId="2" sqref="C35 C23:F23 C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -32912,16 +32909,16 @@
       <c r="B13" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="106" t="s">
+      <c r="C13" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D13" s="106" t="s">
+      <c r="D13" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="106" t="s">
+      <c r="E13" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="106" t="s">
+      <c r="F13" s="10" t="s">
         <v>99</v>
       </c>
       <c r="G13" s="11"/>
@@ -33119,7 +33116,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="oL4RCMZz+ptelxGxmw0ncxtnhzDeKbNT7wopTTk+MnC02N8rE77bl/LByGmJe7Q/cW2tEz4tU0AFsg1eHR6rsA==" saltValue="8KmH41yiLh3RYiu3at1IeA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="wLhQTDa5ZLdiJhtkrrbF70/tl+CSoQ5uC6U+Tvz11zPw6g7ZpBcjZNYngzQ/gMQlkhrECJjfvsvnkt6chZJsOQ==" saltValue="HowjnO0HsyYMvGT3rAYRWA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -33374,16 +33371,16 @@
         <v>125</v>
       </c>
       <c r="L13" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="M13" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="M13" s="10" t="s">
+      <c r="N13" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="N13" s="10" t="s">
+      <c r="O13" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="O13" s="10" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -33476,7 +33473,7 @@
       <c r="G17" s="2"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8j7TxMk9EQxXUJ+Zhxu8++3qctG1QR3ncMhuaW3b5j1kN0vxczG3Vk/OhJJZieMn0QuwFx6D1EibgYtjRKr0Pw==" saltValue="H9ImAdU4fId9JrxPOJujpg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="oCxkF9eXSd9VInGRSEaC68oupkgvuYHflUqtXTDnSca+Fnm5x9/tK7RNIicZTt61u3uQ9XpQdIPY0iXVZ3e8ug==" saltValue="zA1Js/s6185ZfBz+vSEfQg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -33582,7 +33579,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DPH6L+iglYEuLiI88/9guVKq1je6+54d0s1E1q2BqHnhW5xCx28/JCMfHeJbsLN+WfQRYlk+MGJlInI7cuU3lQ==" saltValue="+1CK0Fq7r0C3mksjUxeOiw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Wy13Rr3zPMTlxbk8UOeNp5ydFnjIwtDbYAMFH+RxWfdfh13xYwCTn4mPU5dOBdjBaw/KQJb7Ci2RAZM3i0+oGw==" saltValue="CzQYVFtcKK7o20moDcKUfQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
@@ -33789,7 +33786,7 @@
       <c r="K14" s="104"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/wEyC5afRpRrJ8jzP+MRkcj+SJ3GII55o5tYJuwJDFvGBwJ17V1JAf7z5wbdST3z+g/z8TU5XPiIbEYDQtJGlQ==" saltValue="gTNsXfB6TXZi7euFR4NJYw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="z3S6EJ4R8glPcRt7sj9l+VoiWr4tf25b97jFu+8IUa/D2HaOvwN++gk/PwflUIZh0dchqNM1IaqDWdxUYveuYw==" saltValue="Bk3JeswRhg4vAty4OtvWsg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="193" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -33870,7 +33867,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DLksHDO2fixTCKdFQ713QJqwAh6hqpToirvg/zQem5UzbO+cs5YnmXwdVMViZq09ORwtfKBWAz4Ycl/GZg0ACQ==" saltValue="2mZla5mvWgj5b5NmfiWrdA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="xEjJNYtsLzKruwgcW101Mx+UqxAonlMnO+RDL1QSSqZka7MMoyEhzUypjBQBHSMPAs84ZbTdLt8/ALPHsAQuEQ==" saltValue="l1GNZPF6f9CmW4Klk58/8w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -34131,7 +34128,7 @@
       <c r="E21" s="42"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="uOa7KianIMYvLtAQ2rhHkfN1R5I4vrtrbmk1HMU2p5afXp8BdnoxLhx75YvBSVCvGIfaeAwBaEthHt4/jxN88w==" saltValue="QS6hh1v/Tjp+nPFEbSr6KA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="aGkgulUa9+sxx2d05bPqwKdA2vLQXVDcG4IyCd9S7r4siveRYvxM9L1jQMYOgszOKUZotKrgIbqkSKalfiQkaA==" saltValue="Ij9isrBXBLx71jJud3Hcpw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -34195,7 +34192,7 @@
       <c r="D3" s="42"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="qgUo1m25EeniydYKme+9NTxi5NEeEjiKHotN90MLUPMKExoFAhL8dzuHUyD22GHwm0hqUyPK8SuVLbKUNEN3FA==" saltValue="Zo8loqkZf1EgatubTUawyg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ZKX+A1FDpoEGLAgB9+nFk07l7ltekerq6N7yE/PPS8ud7P3CWIm5P7OsqYwasH8gGPeV/Vtjn8SL4bK6k5NJew==" saltValue="3u5wmBxyZ5cSW1Fh7NLjLw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>